<commit_message>
ran calib and meas on 1k resistor with offset applied to Irms
</commit_message>
<xml_diff>
--- a/software/ble/Calib_and_Measure.xlsx
+++ b/software/ble/Calib_and_Measure.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
-    <sheet name="Measurement" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Measurement - offset on current" sheetId="2" r:id="rId2"/>
+    <sheet name="Measurement - offset on Irms" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Power</t>
   </si>
@@ -35,13 +35,42 @@
   <si>
     <t>Pct Error</t>
   </si>
+  <si>
+    <t>Set to 100 W, re-scale</t>
+  </si>
+  <si>
+    <t>Set to ?? W, re-scale</t>
+  </si>
+  <si>
+    <t>Var</t>
+  </si>
+  <si>
+    <t>R17 = 1k</t>
+  </si>
+  <si>
+    <t>R17 = 4.99k</t>
+  </si>
+  <si>
+    <t>App P</t>
+  </si>
+  <si>
+    <t>True scaled</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -69,11 +98,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -231,11 +263,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68733568"/>
-        <c:axId val="68732032"/>
+        <c:axId val="61034496"/>
+        <c:axId val="61036032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68733568"/>
+        <c:axId val="61034496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -245,12 +277,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68732032"/>
+        <c:crossAx val="61036032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68732032"/>
+        <c:axId val="61036032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -261,7 +293,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68733568"/>
+        <c:crossAx val="61034496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -303,7 +335,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Measurement!$C$1</c:f>
+              <c:f>'Measurement - offset on current'!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -319,7 +351,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Measurement!$A$2:$A$22</c:f>
+              <c:f>'Measurement - offset on current'!$A$5:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -391,7 +423,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Measurement!$C$2:$C$22</c:f>
+              <c:f>'Measurement - offset on current'!$C$5:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -468,7 +500,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Measurement!$B$1</c:f>
+              <c:f>'Measurement - offset on current'!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -485,10 +517,15 @@
           <c:marker>
             <c:symbol val="triangle"/>
             <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Measurement!$A$2:$A$22</c:f>
+              <c:f>'Measurement - offset on current'!$A$5:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -560,7 +597,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Measurement!$B$2:$B$22</c:f>
+              <c:f>'Measurement - offset on current'!$B$5:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -640,8 +677,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="51902720"/>
-        <c:axId val="51901184"/>
+        <c:axId val="60979456"/>
+        <c:axId val="60989440"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -651,7 +688,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Measurement!$D$1</c:f>
+              <c:f>'Measurement - offset on current'!$D$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -667,7 +704,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Measurement!$A$2:$A$22</c:f>
+              <c:f>'Measurement - offset on current'!$A$5:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -739,7 +776,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Measurement!$D$2:$D$22</c:f>
+              <c:f>'Measurement - offset on current'!$D$5:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -819,11 +856,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67794816"/>
-        <c:axId val="66633728"/>
+        <c:axId val="60992512"/>
+        <c:axId val="60990976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51902720"/>
+        <c:axId val="60979456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -833,12 +870,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51901184"/>
+        <c:crossAx val="60989440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51901184"/>
+        <c:axId val="60989440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -851,12 +888,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51902720"/>
+        <c:crossAx val="60979456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66633728"/>
+        <c:axId val="60990976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -868,12 +905,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67794816"/>
+        <c:crossAx val="60992512"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67794816"/>
+        <c:axId val="60992512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -883,7 +920,1404 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66633728"/>
+        <c:crossAx val="60990976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Measurement - offset on Irms'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TRUE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Measurement - offset on Irms'!$A$5:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Measurement - offset on Irms'!$D$5:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>4.3985855172413793</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0232882758620692</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.5005484482758611</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.353623620689653</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.536592706896549</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>74.696700000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99.879592758620689</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>150.35435224137933</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>199.88797293103448</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250.70946775862069</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>301.63002982758621</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>352.71900620689655</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>402.29225379310344</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>451.66736689655175</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>506.56052534482757</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>558.5014799999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>610.42262120689657</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>662.60133724137938</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>708.76667172413806</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>760.07359603448288</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>813.25289120689649</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>871.91060482758621</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>925.0007394827586</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>966.84674224137939</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1030.2101498275863</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1081.0316446551724</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1134.993571034483</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1189.0545646551723</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1243.0363044827586</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Measurement - offset on Irms'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Measurement - offset on Irms'!$A$5:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Measurement - offset on Irms'!$B$5:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="66875392"/>
+        <c:axId val="66754816"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Measurement - offset on Irms'!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Measurement - offset on Irms'!$A$5:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Measurement - offset on Irms'!$E$5:$E$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.39600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.50900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.67200000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.77200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.88800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.91500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.92400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.93600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.95399999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.96899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.97099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.96599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.96399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.96599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.98599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.98599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.97399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.98599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.98499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.98399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.98299999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="139342592"/>
+        <c:axId val="139623040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="66875392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66754816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="66754816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66875392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="139623040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.2"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="139342592"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="139342592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="139623040"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Measurement - offset on Irms'!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Abs Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Measurement - offset on Irms'!$A$5:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Measurement - offset on Irms'!$G$5:$G$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2.3985855172413793</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0232882758620692</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49945155172413891</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64637637931034675</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.46340729310345097</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.30329999999999302</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12040724137931136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35435224137933119</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11202706896551717</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.70946775862068989</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6300298275862133</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.7190062068965517</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2922537931034412</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.667366896551755</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.5605253448275676</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.5014799999999013</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.422621206896565</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.601337241379383</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.7666717241380638</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.073596034482875</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13.252891206896493</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.910604827586212</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>25.000739482758604</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16.846742241379388</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>30.210149827586292</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>31.031644655172386</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>34.993571034483011</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>39.054564655172271</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43.036304482758624</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="165036800"/>
+        <c:axId val="139750400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="165036800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="139750400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="139750400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="165036800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Measurement - offset on Irms'!$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pct Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Measurement - offset on Irms'!$A$5:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Measurement - offset on Irms'!$H$5:$H$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>122.00000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.1000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2333333333333367</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0000000000002274E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.53333333333334099</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.81999999999999318</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1800000000000068</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.885000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2279999999999973</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4900000000000091</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7257142857142915</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.519999999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3155555555555591</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.2659999999999969</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5018181818181802</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.6949999999999932</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.8984615384615435</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.2057142857142935</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.2973333333333357</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.613749999999996</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.5435294117647063</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.7455555555555597</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.7315789473684258</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.9910000000000085</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.9247619047619078</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.1527272727272786</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.3695652173913047</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5616666666666674</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="73312128"/>
+        <c:axId val="73310592"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="73312128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73310592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="73310592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="22"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73312128"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -945,13 +2379,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -966,6 +2400,101 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1263,7 +2792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
@@ -1389,529 +2918,548 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>1.15E-2</v>
+      </c>
+      <c r="E2">
+        <v>3.19E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="b">
+      <c r="C4" t="b">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>7.66</v>
-      </c>
-      <c r="D2">
-        <v>0.193</v>
-      </c>
-      <c r="E2">
-        <f>ABS(B2-C2)</f>
-        <v>2.34</v>
-      </c>
-      <c r="F2">
-        <f>ABS(B2-C2)/B2*100</f>
-        <v>23.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="D3">
-        <v>0.38800000000000001</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E23" si="0">ABS(B3-C3)</f>
-        <v>3.6000000000000014</v>
-      </c>
-      <c r="F3">
-        <f>ABS(B3-C3)/B3*100</f>
-        <v>18.000000000000007</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>26.54</v>
-      </c>
-      <c r="D4">
-        <v>0.55900000000000005</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>3.4600000000000009</v>
-      </c>
-      <c r="F4">
-        <f>ABS(B4-C4)/B4*100</f>
-        <v>11.533333333333335</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>37.18</v>
+        <v>7.66</v>
       </c>
       <c r="D5">
-        <v>0.69599999999999995</v>
+        <v>0.193</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>2.8200000000000003</v>
+        <f>ABS(B5-C5)</f>
+        <v>2.34</v>
       </c>
       <c r="F5">
-        <f>ABS(B5-C5)/B5*100</f>
-        <v>7.0500000000000007</v>
+        <f t="shared" ref="F5:F26" si="0">ABS(B5-C5)/B5*100</f>
+        <v>23.4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B6">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>47.31</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="D6">
-        <v>0.78300000000000003</v>
+        <v>0.38800000000000001</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>2.6899999999999977</v>
+        <f t="shared" ref="E6:E26" si="1">ABS(B6-C6)</f>
+        <v>3.6000000000000014</v>
       </c>
       <c r="F6">
-        <f>ABS(B6-C6)/B6*100</f>
-        <v>5.3799999999999955</v>
+        <f t="shared" si="0"/>
+        <v>18.000000000000007</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="B7">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C7">
-        <v>72.849999999999994</v>
+        <v>26.54</v>
       </c>
       <c r="D7">
-        <v>0.89300000000000002</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>2.1500000000000057</v>
+        <f t="shared" si="1"/>
+        <v>3.4600000000000009</v>
       </c>
       <c r="F7">
-        <f>ABS(B7-C7)/B7*100</f>
-        <v>2.8666666666666742</v>
+        <f t="shared" si="0"/>
+        <v>11.533333333333335</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="B8">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="C8">
-        <v>98.07</v>
+        <v>37.18</v>
       </c>
       <c r="D8">
-        <v>0.94</v>
+        <v>0.69599999999999995</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>1.9300000000000068</v>
+        <f t="shared" si="1"/>
+        <v>2.8200000000000003</v>
       </c>
       <c r="F8">
-        <f>ABS(B8-C8)/B8*100</f>
-        <v>1.9300000000000068</v>
+        <f t="shared" si="0"/>
+        <v>7.0500000000000007</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>125</v>
+        <v>50</v>
       </c>
       <c r="B9">
-        <v>125</v>
+        <v>50</v>
       </c>
       <c r="C9">
-        <v>123.4</v>
+        <v>47.31</v>
       </c>
       <c r="D9">
-        <v>0.96799999999999997</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
-        <v>1.5999999999999943</v>
+        <f t="shared" si="1"/>
+        <v>2.6899999999999977</v>
       </c>
       <c r="F9">
-        <f>ABS(B9-C9)/B9*100</f>
-        <v>1.2799999999999954</v>
+        <f t="shared" si="0"/>
+        <v>5.3799999999999955</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="B10">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="C10">
-        <v>148.69999999999999</v>
+        <v>72.849999999999994</v>
       </c>
       <c r="D10">
-        <v>0.98</v>
+        <v>0.89300000000000002</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>1.3000000000000114</v>
+        <f t="shared" si="1"/>
+        <v>2.1500000000000057</v>
       </c>
       <c r="F10">
-        <f>ABS(B10-C10)/B10*100</f>
-        <v>0.86666666666667425</v>
+        <f t="shared" si="0"/>
+        <v>2.8666666666666742</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>175</v>
+        <v>100</v>
       </c>
       <c r="B11">
-        <v>175</v>
+        <v>100</v>
       </c>
       <c r="C11">
-        <v>174.63</v>
+        <v>98.07</v>
       </c>
       <c r="D11">
-        <v>0.98699999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>0.37000000000000455</v>
+        <f t="shared" si="1"/>
+        <v>1.9300000000000068</v>
       </c>
       <c r="F11">
-        <f>ABS(B11-C11)/B11*100</f>
-        <v>0.21142857142857405</v>
+        <f t="shared" si="0"/>
+        <v>1.9300000000000068</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>200</v>
+        <v>125</v>
       </c>
       <c r="B12">
-        <v>200</v>
+        <v>125</v>
       </c>
       <c r="C12">
-        <v>199.85</v>
+        <v>123.4</v>
       </c>
       <c r="D12">
-        <v>0.99199999999999999</v>
+        <v>0.96799999999999997</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>0.15000000000000568</v>
+        <f t="shared" si="1"/>
+        <v>1.5999999999999943</v>
       </c>
       <c r="F12">
-        <f>ABS(B12-C12)/B12*100</f>
-        <v>7.5000000000002842E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.2799999999999954</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>225</v>
+        <v>150</v>
       </c>
       <c r="B13">
-        <v>225</v>
+        <v>150</v>
       </c>
       <c r="C13">
-        <v>224.76</v>
+        <v>148.69999999999999</v>
       </c>
       <c r="D13">
-        <v>0.98799999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>0.24000000000000909</v>
+        <f t="shared" si="1"/>
+        <v>1.3000000000000114</v>
       </c>
       <c r="F13">
-        <f>ABS(B13-C13)/B13*100</f>
-        <v>0.10666666666667071</v>
+        <f t="shared" si="0"/>
+        <v>0.86666666666667425</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>250</v>
+        <v>175</v>
       </c>
       <c r="B14">
-        <v>250</v>
+        <v>175</v>
       </c>
       <c r="C14">
-        <v>250.21</v>
+        <v>174.63</v>
       </c>
       <c r="D14">
-        <v>0.98899999999999999</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>0.21000000000000796</v>
+        <f t="shared" si="1"/>
+        <v>0.37000000000000455</v>
       </c>
       <c r="F14">
-        <f>ABS(B14-C14)/B14*100</f>
-        <v>8.4000000000003183E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.21142857142857405</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>275</v>
+        <v>200</v>
       </c>
       <c r="B15">
-        <v>275</v>
+        <v>200</v>
       </c>
       <c r="C15">
-        <v>275.52</v>
+        <v>199.85</v>
       </c>
       <c r="D15">
-        <v>0.98699999999999999</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>0.51999999999998181</v>
+        <f t="shared" si="1"/>
+        <v>0.15000000000000568</v>
       </c>
       <c r="F15">
-        <f>ABS(B15-C15)/B15*100</f>
-        <v>0.18909090909090248</v>
+        <f t="shared" si="0"/>
+        <v>7.5000000000002842E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>300</v>
+        <v>225</v>
       </c>
       <c r="B16">
-        <v>300</v>
+        <v>225</v>
       </c>
       <c r="C16">
-        <v>301.61</v>
+        <v>224.76</v>
       </c>
       <c r="D16">
-        <v>0.99</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>1.6100000000000136</v>
+        <f t="shared" si="1"/>
+        <v>0.24000000000000909</v>
       </c>
       <c r="F16">
-        <f>ABS(B16-C16)/B16*100</f>
-        <v>0.53666666666667118</v>
+        <f t="shared" si="0"/>
+        <v>0.10666666666667071</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>325</v>
+        <v>250</v>
       </c>
       <c r="B17">
-        <v>325</v>
+        <v>250</v>
       </c>
       <c r="C17">
-        <v>326.54000000000002</v>
+        <v>250.21</v>
       </c>
       <c r="D17">
-        <v>0.98799999999999999</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>1.5400000000000205</v>
+        <f t="shared" si="1"/>
+        <v>0.21000000000000796</v>
       </c>
       <c r="F17">
-        <f>ABS(B17-C17)/B17*100</f>
-        <v>0.47384615384616013</v>
+        <f t="shared" si="0"/>
+        <v>8.4000000000003183E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>350</v>
+        <v>275</v>
       </c>
       <c r="B18">
-        <v>350</v>
+        <v>275</v>
       </c>
       <c r="C18">
-        <v>351.69</v>
+        <v>275.52</v>
       </c>
       <c r="D18">
-        <v>0.99199999999999999</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>1.6899999999999977</v>
+        <f t="shared" si="1"/>
+        <v>0.51999999999998181</v>
       </c>
       <c r="F18">
-        <f>ABS(B18-C18)/B18*100</f>
-        <v>0.48285714285714215</v>
+        <f t="shared" si="0"/>
+        <v>0.18909090909090248</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>375</v>
+        <v>300</v>
       </c>
       <c r="B19">
-        <v>375</v>
+        <v>300</v>
       </c>
       <c r="C19">
-        <v>377.95</v>
+        <v>301.61</v>
       </c>
       <c r="D19">
-        <v>0.99299999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>2.9499999999999886</v>
+        <f t="shared" si="1"/>
+        <v>1.6100000000000136</v>
       </c>
       <c r="F19">
-        <f>ABS(B19-C19)/B19*100</f>
-        <v>0.78666666666666363</v>
+        <f t="shared" si="0"/>
+        <v>0.53666666666667118</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>400</v>
+        <v>325</v>
       </c>
       <c r="B20">
-        <v>400</v>
+        <v>325</v>
       </c>
       <c r="C20">
-        <v>403.1</v>
+        <v>326.54000000000002</v>
       </c>
       <c r="D20">
-        <v>0.99199999999999999</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
-        <v>3.1000000000000227</v>
+        <f t="shared" si="1"/>
+        <v>1.5400000000000205</v>
       </c>
       <c r="F20">
-        <f>ABS(B20-C20)/B20*100</f>
-        <v>0.77500000000000568</v>
+        <f t="shared" si="0"/>
+        <v>0.47384615384616013</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>425</v>
+        <v>350</v>
       </c>
       <c r="B21">
-        <v>425</v>
+        <v>350</v>
       </c>
       <c r="C21">
-        <v>429.48</v>
+        <v>351.69</v>
       </c>
       <c r="D21">
-        <v>0.99399999999999999</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
-        <v>4.4800000000000182</v>
+        <f t="shared" si="1"/>
+        <v>1.6899999999999977</v>
       </c>
       <c r="F21">
-        <f>ABS(B21-C21)/B21*100</f>
-        <v>1.0541176470588278</v>
+        <f t="shared" si="0"/>
+        <v>0.48285714285714215</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>450</v>
+        <v>375</v>
       </c>
       <c r="B22">
-        <v>450</v>
+        <v>375</v>
       </c>
       <c r="C22">
-        <v>454.05</v>
+        <v>377.95</v>
       </c>
       <c r="D22">
-        <v>0.99399999999999999</v>
+        <v>0.99299999999999999</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
-        <v>4.0500000000000114</v>
+        <f t="shared" si="1"/>
+        <v>2.9499999999999886</v>
       </c>
       <c r="F22">
-        <f>ABS(B22-C22)/B22*100</f>
-        <v>0.90000000000000258</v>
+        <f t="shared" si="0"/>
+        <v>0.78666666666666363</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
+        <v>400</v>
+      </c>
+      <c r="B23">
+        <v>400</v>
+      </c>
+      <c r="C23">
+        <v>403.1</v>
+      </c>
+      <c r="D23">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>3.1000000000000227</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0.77500000000000568</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>425</v>
+      </c>
+      <c r="B24">
+        <v>425</v>
+      </c>
+      <c r="C24">
+        <v>429.48</v>
+      </c>
+      <c r="D24">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>4.4800000000000182</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>1.0541176470588278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>450</v>
+      </c>
+      <c r="B25">
+        <v>450</v>
+      </c>
+      <c r="C25">
+        <v>454.05</v>
+      </c>
+      <c r="D25">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>4.0500000000000114</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0.90000000000000258</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>475</v>
       </c>
-      <c r="B23">
+      <c r="B26">
         <v>475</v>
       </c>
-      <c r="C23">
+      <c r="C26">
         <v>449.12</v>
       </c>
-      <c r="D23">
+      <c r="D26">
         <v>0.91900000000000004</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
+      <c r="E26">
+        <f t="shared" si="1"/>
         <v>25.879999999999995</v>
       </c>
-      <c r="F23">
-        <f>ABS(B23-C23)/B23*100</f>
+      <c r="F26">
+        <f t="shared" si="0"/>
         <v>5.4484210526315779</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E24">
-        <f>AVERAGE(E2:E22)</f>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f>AVERAGE(E5:E25)</f>
         <v>2.0380952380952428</v>
       </c>
-      <c r="F24">
-        <f>AVERAGEIF(F2:F22,"&lt;100")</f>
+      <c r="F27">
+        <f>AVERAGEIF(F5:F25,"&lt;100")</f>
         <v>3.713428909092777</v>
       </c>
-      <c r="G24">
-        <f>AVERAGE(F4:F22)</f>
+      <c r="G27">
+        <f>AVERAGE(F7:F25)</f>
         <v>1.9253687942604374</v>
       </c>
     </row>
@@ -1923,12 +3471,1065 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.6099999999999998E-5</v>
+      </c>
+      <c r="H2">
+        <v>5.7459000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <f>A5</f>
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="D5" s="3">
+        <f>C5*H$2/E$2</f>
+        <v>4.3985855172413793</v>
+      </c>
+      <c r="E5">
+        <v>0.02</v>
+      </c>
+      <c r="F5">
+        <v>3.79</v>
+      </c>
+      <c r="G5">
+        <f>ABS(B5-D5)</f>
+        <v>2.3985855172413793</v>
+      </c>
+      <c r="H5" s="3">
+        <f>ABS(B5-C5)/B5*100</f>
+        <v>122.00000000000001</v>
+      </c>
+      <c r="I5">
+        <f>C5/E5</f>
+        <v>222.00000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ref="B6:B33" si="0">A6</f>
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>6.08</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ref="D6:D33" si="1">C6*H$2/E$2</f>
+        <v>6.0232882758620692</v>
+      </c>
+      <c r="E6">
+        <v>0.03</v>
+      </c>
+      <c r="F6">
+        <v>5.29</v>
+      </c>
+      <c r="G6">
+        <f>ABS(B6-D6)</f>
+        <v>1.0232882758620692</v>
+      </c>
+      <c r="H6" s="3">
+        <f>ABS(B6-C6)/B6*100</f>
+        <v>21.6</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I33" si="2">C6/E6</f>
+        <v>202.66666666666669</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>9.59</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="1"/>
+        <v>9.5005484482758611</v>
+      </c>
+      <c r="E7">
+        <v>0.05</v>
+      </c>
+      <c r="F7">
+        <v>13.44</v>
+      </c>
+      <c r="G7">
+        <f>ABS(B7-D7)</f>
+        <v>0.49945155172413891</v>
+      </c>
+      <c r="H7" s="3">
+        <f>ABS(B7-C7)/B7*100</f>
+        <v>4.1000000000000014</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>191.79999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>29.63</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="1"/>
+        <v>29.353623620689653</v>
+      </c>
+      <c r="E8">
+        <v>0.15</v>
+      </c>
+      <c r="F8">
+        <v>50.25</v>
+      </c>
+      <c r="G8">
+        <f>ABS(B8-D8)</f>
+        <v>0.64637637931034675</v>
+      </c>
+      <c r="H8" s="3">
+        <f>ABS(B8-C8)/B8*100</f>
+        <v>1.2333333333333367</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>197.53333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="C9">
+        <v>50.003</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="1"/>
+        <v>49.536592706896549</v>
+      </c>
+      <c r="E9">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="F9">
+        <v>10.52</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:G33" si="3">ABS(B9-D9)</f>
+        <v>0.46340729310345097</v>
+      </c>
+      <c r="H9" s="3">
+        <f>ABS(B9-C9)/B9*100</f>
+        <v>6.0000000000002274E-3</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>187.98120300751879</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>75</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="C10">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="1"/>
+        <v>74.696700000000007</v>
+      </c>
+      <c r="E10">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="F10">
+        <v>1.94</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>0.30329999999999302</v>
+      </c>
+      <c r="H10" s="3">
+        <f>ABS(B10-C10)/B10*100</f>
+        <v>0.53333333333334099</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>190.40404040404042</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>100.82</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="1"/>
+        <v>99.879592758620689</v>
+      </c>
+      <c r="E11">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="F11">
+        <v>1.55</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>0.12040724137931136</v>
+      </c>
+      <c r="H11" s="3">
+        <f>ABS(B11-C11)/B11*100</f>
+        <v>0.81999999999999318</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>198.0746561886051</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>150</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C12">
+        <v>151.77000000000001</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="1"/>
+        <v>150.35435224137933</v>
+      </c>
+      <c r="E12">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="F12">
+        <v>2.04</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>0.35435224137933119</v>
+      </c>
+      <c r="H12" s="3">
+        <f>ABS(B12-C12)/B12*100</f>
+        <v>1.1800000000000068</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>225.84821428571428</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>200</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="C13">
+        <v>201.77</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="1"/>
+        <v>199.88797293103448</v>
+      </c>
+      <c r="E13">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="F13">
+        <v>26.33</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>0.11202706896551717</v>
+      </c>
+      <c r="H13" s="3">
+        <f>ABS(B13-C13)/B13*100</f>
+        <v>0.885000000000005</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>261.36010362694299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>250</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="C14">
+        <v>253.07</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="1"/>
+        <v>250.70946775862069</v>
+      </c>
+      <c r="E14">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="F14">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>0.70946775862068989</v>
+      </c>
+      <c r="H14" s="3">
+        <f>ABS(B14-C14)/B14*100</f>
+        <v>1.2279999999999973</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>298.43160377358492</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>300</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="C15">
+        <v>304.47000000000003</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="1"/>
+        <v>301.63002982758621</v>
+      </c>
+      <c r="E15">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="F15">
+        <v>2.15</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>1.6300298275862133</v>
+      </c>
+      <c r="H15" s="3">
+        <f>ABS(B15-C15)/B15*100</f>
+        <v>1.4900000000000091</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>342.87162162162167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>350</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="C16">
+        <v>356.04</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="1"/>
+        <v>352.71900620689655</v>
+      </c>
+      <c r="E16">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="F16">
+        <v>3.3</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>2.7190062068965517</v>
+      </c>
+      <c r="H16" s="3">
+        <f>ABS(B16-C16)/B16*100</f>
+        <v>1.7257142857142915</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>389.11475409836066</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>400</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="C17">
+        <v>406.08</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="1"/>
+        <v>402.29225379310344</v>
+      </c>
+      <c r="E17">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="F17">
+        <v>473.89</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>2.2922537931034412</v>
+      </c>
+      <c r="H17" s="3">
+        <f>ABS(B17-C17)/B17*100</f>
+        <v>1.519999999999996</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>439.48051948051943</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>450</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+      <c r="C18">
+        <v>455.92</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="1"/>
+        <v>451.66736689655175</v>
+      </c>
+      <c r="E18">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="F18">
+        <v>798.47</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>1.667366896551755</v>
+      </c>
+      <c r="H18" s="3">
+        <f>ABS(B18-C18)/B18*100</f>
+        <v>1.3155555555555591</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>487.09401709401709</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>500</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="C19">
+        <v>511.33</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="1"/>
+        <v>506.56052534482757</v>
+      </c>
+      <c r="E19">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="F19">
+        <v>3.9</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>6.5605253448275676</v>
+      </c>
+      <c r="H19" s="3">
+        <f>ABS(B19-C19)/B19*100</f>
+        <v>2.2659999999999969</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>535.98532494758911</v>
+      </c>
+      <c r="J19">
+        <f>AVERAGE(H6:H19)</f>
+        <v>2.8502097505668957</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>550</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>550</v>
+      </c>
+      <c r="C20">
+        <v>563.76</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="1"/>
+        <v>558.5014799999999</v>
+      </c>
+      <c r="E20">
+        <v>0.96</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>8.5014799999999013</v>
+      </c>
+      <c r="H20" s="3">
+        <f>ABS(B20-C20)/B20*100</f>
+        <v>2.5018181818181802</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>587.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>600</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="C21">
+        <v>616.16999999999996</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="1"/>
+        <v>610.42262120689657</v>
+      </c>
+      <c r="E21">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="F21">
+        <v>3.66</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>10.422621206896565</v>
+      </c>
+      <c r="H21" s="3">
+        <f>ABS(B21-C21)/B21*100</f>
+        <v>2.6949999999999932</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>635.88235294117646</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>650</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>650</v>
+      </c>
+      <c r="C22">
+        <v>668.84</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="1"/>
+        <v>662.60133724137938</v>
+      </c>
+      <c r="E22">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="F22">
+        <v>5.29</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>12.601337241379383</v>
+      </c>
+      <c r="H22" s="3">
+        <f>ABS(B22-C22)/B22*100</f>
+        <v>2.8984615384615435</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>688.81565396498456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>700</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="C23">
+        <v>715.44</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="1"/>
+        <v>708.76667172413806</v>
+      </c>
+      <c r="E23">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="F23">
+        <v>2011.73</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>8.7666717241380638</v>
+      </c>
+      <c r="H23" s="3">
+        <f>ABS(B23-C23)/B23*100</f>
+        <v>2.2057142857142935</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>740.62111801242247</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>750</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+      <c r="C24">
+        <v>767.23</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="1"/>
+        <v>760.07359603448288</v>
+      </c>
+      <c r="E24">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="F24">
+        <v>2300.21</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>10.073596034482875</v>
+      </c>
+      <c r="H24" s="3">
+        <f>ABS(B24-C24)/B24*100</f>
+        <v>2.2973333333333357</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>795.88174273858931</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>800</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="C25">
+        <v>820.91</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="1"/>
+        <v>813.25289120689649</v>
+      </c>
+      <c r="E25">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="F25">
+        <v>2615.87</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>13.252891206896493</v>
+      </c>
+      <c r="H25" s="3">
+        <f>ABS(B25-C25)/B25*100</f>
+        <v>2.613749999999996</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>849.80331262939956</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>850</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>850</v>
+      </c>
+      <c r="C26">
+        <v>880.12</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="1"/>
+        <v>871.91060482758621</v>
+      </c>
+      <c r="E26">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="F26">
+        <v>9.31</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>21.910604827586212</v>
+      </c>
+      <c r="H26" s="3">
+        <f>ABS(B26-C26)/B26*100</f>
+        <v>3.5435294117647063</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>892.61663286004057</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>900</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="C27">
+        <v>933.71</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="1"/>
+        <v>925.0007394827586</v>
+      </c>
+      <c r="E27">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="F27">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>25.000739482758604</v>
+      </c>
+      <c r="H27" s="3">
+        <f>ABS(B27-C27)/B27*100</f>
+        <v>3.7455555555555597</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>946.96754563894524</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>950</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>950</v>
+      </c>
+      <c r="C28">
+        <v>975.95</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="1"/>
+        <v>966.84674224137939</v>
+      </c>
+      <c r="E28">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="F28">
+        <v>4137.1499999999996</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>16.846742241379388</v>
+      </c>
+      <c r="H28" s="3">
+        <f>ABS(B28-C28)/B28*100</f>
+        <v>2.7315789473684258</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>1002.0020533880904</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1000</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="C29">
+        <v>1039.9100000000001</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="1"/>
+        <v>1030.2101498275863</v>
+      </c>
+      <c r="E29">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="F29">
+        <v>11.02</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>30.210149827586292</v>
+      </c>
+      <c r="H29" s="3">
+        <f>ABS(B29-C29)/B29*100</f>
+        <v>3.9910000000000085</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>1054.6754563894524</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1050</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>1050</v>
+      </c>
+      <c r="C30">
+        <v>1091.21</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="1"/>
+        <v>1081.0316446551724</v>
+      </c>
+      <c r="E30">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="F30">
+        <v>11.68</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>31.031644655172386</v>
+      </c>
+      <c r="H30" s="3">
+        <f>ABS(B30-C30)/B30*100</f>
+        <v>3.9247619047619078</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>1107.8274111675128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1100</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="C31">
+        <v>1145.68</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="1"/>
+        <v>1134.993571034483</v>
+      </c>
+      <c r="E31">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="F31">
+        <v>10.06</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>34.993571034483011</v>
+      </c>
+      <c r="H31" s="3">
+        <f>ABS(B31-C31)/B31*100</f>
+        <v>4.1527272727272786</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>1163.1269035532996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1150</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>1150</v>
+      </c>
+      <c r="C32">
+        <v>1200.25</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="1"/>
+        <v>1189.0545646551723</v>
+      </c>
+      <c r="E32">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="F32">
+        <v>11.93</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>39.054564655172271</v>
+      </c>
+      <c r="H32" s="3">
+        <f>ABS(B32-C32)/B32*100</f>
+        <v>4.3695652173913047</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>1219.7662601626016</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1200</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="C33">
+        <v>1254.74</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="1"/>
+        <v>1243.0363044827586</v>
+      </c>
+      <c r="E33">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="F33">
+        <v>14.47</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="3"/>
+        <v>43.036304482758624</v>
+      </c>
+      <c r="H33" s="3">
+        <f>ABS(B33-C33)/B33*100</f>
+        <v>4.5616666666666674</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>1276.439471007121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <f>AVERAGE(G6:G33)</f>
+        <v>11.600149232142872</v>
+      </c>
+      <c r="H34">
+        <f>AVERAGEIF(H5:H33,"&lt;100")</f>
+        <v>3.0762642436964192</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added copy-able data fields in calib and measure
</commit_message>
<xml_diff>
--- a/software/ble/Calib_and_Measure.xlsx
+++ b/software/ble/Calib_and_Measure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22160" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -190,8 +190,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -207,9 +209,11 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -476,11 +480,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2138647432"/>
-        <c:axId val="-2138644456"/>
+        <c:axId val="2123876680"/>
+        <c:axId val="2123873784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2138647432"/>
+        <c:axId val="2123876680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,12 +494,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2138644456"/>
+        <c:crossAx val="2123873784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2138644456"/>
+        <c:axId val="2123873784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,7 +510,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2138647432"/>
+        <c:crossAx val="2123876680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -697,11 +701,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135241800"/>
-        <c:axId val="-2135238840"/>
+        <c:axId val="2123466088"/>
+        <c:axId val="2123463128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135241800"/>
+        <c:axId val="2123466088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -711,12 +715,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135238840"/>
+        <c:crossAx val="2123463128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135238840"/>
+        <c:axId val="2123463128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -727,7 +731,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135241800"/>
+        <c:crossAx val="2123466088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -918,11 +922,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135212184"/>
-        <c:axId val="-2135209224"/>
+        <c:axId val="2123436120"/>
+        <c:axId val="2123433160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135212184"/>
+        <c:axId val="2123436120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -932,12 +936,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135209224"/>
+        <c:crossAx val="2123433160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135209224"/>
+        <c:axId val="2123433160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22.0"/>
@@ -949,7 +953,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135212184"/>
+        <c:crossAx val="2123436120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1338,8 +1342,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135573992"/>
-        <c:axId val="-2135571000"/>
+        <c:axId val="2123791752"/>
+        <c:axId val="2123788760"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1517,11 +1521,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135564728"/>
-        <c:axId val="-2135567672"/>
+        <c:axId val="2123782488"/>
+        <c:axId val="2123785432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135573992"/>
+        <c:axId val="2123791752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1531,12 +1535,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135571000"/>
+        <c:crossAx val="2123788760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135571000"/>
+        <c:axId val="2123788760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600.0"/>
@@ -1549,12 +1553,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135573992"/>
+        <c:crossAx val="2123791752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135567672"/>
+        <c:axId val="2123785432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1566,12 +1570,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135564728"/>
+        <c:crossAx val="2123782488"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135564728"/>
+        <c:axId val="2123782488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1581,7 +1585,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135567672"/>
+        <c:crossAx val="2123785432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2080,8 +2084,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135517304"/>
-        <c:axId val="-2135511912"/>
+        <c:axId val="2123733528"/>
+        <c:axId val="2123730968"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2319,11 +2323,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135505640"/>
-        <c:axId val="-2135508584"/>
+        <c:axId val="2123724696"/>
+        <c:axId val="2123727640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135517304"/>
+        <c:axId val="2123733528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2333,12 +2337,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135511912"/>
+        <c:crossAx val="2123730968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135511912"/>
+        <c:axId val="2123730968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2349,12 +2353,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135517304"/>
+        <c:crossAx val="2123733528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135508584"/>
+        <c:axId val="2123727640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -2366,12 +2370,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135505640"/>
+        <c:crossAx val="2123724696"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135505640"/>
+        <c:axId val="2123724696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2381,7 +2385,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135508584"/>
+        <c:crossAx val="2123727640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2646,11 +2650,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135485368"/>
-        <c:axId val="-2135482408"/>
+        <c:axId val="2123704440"/>
+        <c:axId val="2123701480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135485368"/>
+        <c:axId val="2123704440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2660,12 +2664,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135482408"/>
+        <c:crossAx val="2123701480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135482408"/>
+        <c:axId val="2123701480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50.0"/>
@@ -2677,7 +2681,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135485368"/>
+        <c:crossAx val="2123704440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2942,11 +2946,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135455896"/>
-        <c:axId val="-2135452936"/>
+        <c:axId val="2123674984"/>
+        <c:axId val="2123672024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135455896"/>
+        <c:axId val="2123674984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2956,12 +2960,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135452936"/>
+        <c:crossAx val="2123672024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135452936"/>
+        <c:axId val="2123672024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22.0"/>
@@ -2973,7 +2977,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135455896"/>
+        <c:crossAx val="2123674984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3472,8 +3476,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135396600"/>
-        <c:axId val="-2135391208"/>
+        <c:axId val="2123617688"/>
+        <c:axId val="2123615128"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3711,11 +3715,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135384936"/>
-        <c:axId val="-2135387880"/>
+        <c:axId val="2123608856"/>
+        <c:axId val="2123611800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135396600"/>
+        <c:axId val="2123617688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3725,12 +3729,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135391208"/>
+        <c:crossAx val="2123615128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135391208"/>
+        <c:axId val="2123615128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3741,12 +3745,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135396600"/>
+        <c:crossAx val="2123617688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135387880"/>
+        <c:axId val="2123611800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -3758,12 +3762,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135384936"/>
+        <c:crossAx val="2123608856"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135384936"/>
+        <c:axId val="2123608856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3773,7 +3777,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135387880"/>
+        <c:crossAx val="2123611800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4040,11 +4044,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135364328"/>
-        <c:axId val="-2135361368"/>
+        <c:axId val="2123586744"/>
+        <c:axId val="2123583784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135364328"/>
+        <c:axId val="2123586744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4054,12 +4058,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135361368"/>
+        <c:crossAx val="2123583784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135361368"/>
+        <c:axId val="2123583784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4070,7 +4074,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135364328"/>
+        <c:crossAx val="2123586744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4337,11 +4341,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135334200"/>
-        <c:axId val="-2135331240"/>
+        <c:axId val="2123556376"/>
+        <c:axId val="2123553416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135334200"/>
+        <c:axId val="2123556376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4351,12 +4355,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135331240"/>
+        <c:crossAx val="2123553416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135331240"/>
+        <c:axId val="2123553416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22.0"/>
@@ -4368,7 +4372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135334200"/>
+        <c:crossAx val="2123556376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4664,8 +4668,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135274840"/>
-        <c:axId val="-2135269112"/>
+        <c:axId val="2123496008"/>
+        <c:axId val="2123493448"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4807,11 +4811,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135262840"/>
-        <c:axId val="-2135265784"/>
+        <c:axId val="2123487176"/>
+        <c:axId val="2123490120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2135274840"/>
+        <c:axId val="2123496008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4821,12 +4825,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135269112"/>
+        <c:crossAx val="2123493448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135269112"/>
+        <c:axId val="2123493448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4837,12 +4841,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135274840"/>
+        <c:crossAx val="2123496008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135265784"/>
+        <c:axId val="2123490120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -4854,12 +4858,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135262840"/>
+        <c:crossAx val="2123487176"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135262840"/>
+        <c:axId val="2123487176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4869,7 +4873,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135265784"/>
+        <c:crossAx val="2123490120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7416,20 +7420,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:AE38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AE33" sqref="AB5:AE33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -7443,7 +7447,7 @@
         <v>5.7459000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -7469,7 +7473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:31">
       <c r="A5">
         <v>2.2000000000000002</v>
       </c>
@@ -7498,8 +7502,24 @@
         <f t="shared" ref="H5:H33" si="1">C5/D5</f>
         <v>60.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="AB5">
+        <f>B5</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AC5">
+        <f>C5</f>
+        <v>2.41</v>
+      </c>
+      <c r="AD5">
+        <f>H5</f>
+        <v>60.25</v>
+      </c>
+      <c r="AE5">
+        <f>D5</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7528,8 +7548,24 @@
         <f t="shared" si="1"/>
         <v>99.199999999999989</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="AB6">
+        <f t="shared" ref="AB6:AB38" si="4">B6</f>
+        <v>5</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" ref="AC6:AC38" si="5">C6</f>
+        <v>4.96</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" ref="AD6:AD38" si="6">H6</f>
+        <v>99.199999999999989</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" ref="AE6:AE38" si="7">D6</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
       <c r="A7">
         <v>10</v>
       </c>
@@ -7558,8 +7594,24 @@
         <f t="shared" si="1"/>
         <v>155.00000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="AB7">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="5"/>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="6"/>
+        <v>155.00000000000003</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" si="7"/>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31">
       <c r="A8">
         <v>30</v>
       </c>
@@ -7588,8 +7640,24 @@
         <f t="shared" si="1"/>
         <v>184.5625</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="AB8">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="5"/>
+        <v>29.53</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="6"/>
+        <v>184.5625</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" si="7"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31">
       <c r="A9">
         <v>50</v>
       </c>
@@ -7618,8 +7686,24 @@
         <f t="shared" si="1"/>
         <v>202.92</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="AB9">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="5"/>
+        <v>50.73</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="6"/>
+        <v>202.92</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" si="7"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31">
       <c r="A10">
         <v>75.2</v>
       </c>
@@ -7648,8 +7732,24 @@
         <f t="shared" si="1"/>
         <v>211.94444444444446</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="AB10">
+        <f t="shared" si="4"/>
+        <v>75.2</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" si="5"/>
+        <v>76.3</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="6"/>
+        <v>211.94444444444446</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="7"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31">
       <c r="A11">
         <v>100</v>
       </c>
@@ -7678,8 +7778,24 @@
         <f t="shared" si="1"/>
         <v>224.53333333333333</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="AB11">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="AC11">
+        <f t="shared" si="5"/>
+        <v>101.04</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="6"/>
+        <v>224.53333333333333</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" si="7"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31">
       <c r="A12">
         <v>150</v>
       </c>
@@ -7708,8 +7824,24 @@
         <f t="shared" si="1"/>
         <v>254.35593220338984</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="AB12">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="5"/>
+        <v>150.07</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="6"/>
+        <v>254.35593220338984</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="7"/>
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31">
       <c r="A13">
         <v>200</v>
       </c>
@@ -7738,8 +7870,24 @@
         <f t="shared" si="1"/>
         <v>284.85714285714289</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="AB13">
+        <f t="shared" si="4"/>
+        <v>200</v>
+      </c>
+      <c r="AC13">
+        <f t="shared" si="5"/>
+        <v>199.4</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="6"/>
+        <v>284.85714285714289</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="7"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31">
       <c r="A14">
         <v>250</v>
       </c>
@@ -7768,8 +7916,24 @@
         <f t="shared" si="1"/>
         <v>317.84615384615381</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="AB14">
+        <f t="shared" si="4"/>
+        <v>250</v>
+      </c>
+      <c r="AC14">
+        <f t="shared" si="5"/>
+        <v>247.92</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="6"/>
+        <v>317.84615384615381</v>
+      </c>
+      <c r="AE14">
+        <f t="shared" si="7"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31">
       <c r="A15">
         <v>300</v>
       </c>
@@ -7798,8 +7962,24 @@
         <f t="shared" si="1"/>
         <v>358.09638554216872</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="AB15">
+        <f t="shared" si="4"/>
+        <v>300</v>
+      </c>
+      <c r="AC15">
+        <f t="shared" si="5"/>
+        <v>297.22000000000003</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="6"/>
+        <v>358.09638554216872</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" si="7"/>
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31">
       <c r="A16">
         <v>350</v>
       </c>
@@ -7828,8 +8008,24 @@
         <f t="shared" si="1"/>
         <v>403.76744186046511</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="AB16">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="AC16">
+        <f t="shared" si="5"/>
+        <v>347.24</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="6"/>
+        <v>403.76744186046511</v>
+      </c>
+      <c r="AE16">
+        <f t="shared" si="7"/>
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31">
       <c r="A17">
         <v>400</v>
       </c>
@@ -7858,8 +8054,24 @@
         <f t="shared" si="1"/>
         <v>445.8089887640449</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="AB17">
+        <f t="shared" si="4"/>
+        <v>400</v>
+      </c>
+      <c r="AC17">
+        <f t="shared" si="5"/>
+        <v>396.77</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="6"/>
+        <v>445.8089887640449</v>
+      </c>
+      <c r="AE17">
+        <f t="shared" si="7"/>
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31">
       <c r="A18">
         <v>449</v>
       </c>
@@ -7888,8 +8100,24 @@
         <f t="shared" si="1"/>
         <v>496.4111111111111</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="AB18">
+        <f t="shared" si="4"/>
+        <v>449</v>
+      </c>
+      <c r="AC18">
+        <f t="shared" si="5"/>
+        <v>446.77</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="6"/>
+        <v>496.4111111111111</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" si="7"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31">
       <c r="A19">
         <v>499.5</v>
       </c>
@@ -7922,8 +8150,24 @@
         <f>AVERAGE(G6:G19)</f>
         <v>1.3107371036859092</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="AB19">
+        <f t="shared" si="4"/>
+        <v>499.5</v>
+      </c>
+      <c r="AC19">
+        <f t="shared" si="5"/>
+        <v>495.39</v>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="6"/>
+        <v>538.46739130434776</v>
+      </c>
+      <c r="AE19">
+        <f t="shared" si="7"/>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31">
       <c r="A20">
         <v>548.79999999999995</v>
       </c>
@@ -7952,8 +8196,24 @@
         <f t="shared" si="1"/>
         <v>585.97849462365593</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="AB20">
+        <f t="shared" si="4"/>
+        <v>548.79999999999995</v>
+      </c>
+      <c r="AC20">
+        <f t="shared" si="5"/>
+        <v>544.96</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="6"/>
+        <v>585.97849462365593</v>
+      </c>
+      <c r="AE20">
+        <f t="shared" si="7"/>
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31">
       <c r="A21">
         <v>600</v>
       </c>
@@ -7982,8 +8242,24 @@
         <f t="shared" si="1"/>
         <v>634.65957446808522</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="AB21">
+        <f t="shared" si="4"/>
+        <v>600</v>
+      </c>
+      <c r="AC21">
+        <f t="shared" si="5"/>
+        <v>596.58000000000004</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="6"/>
+        <v>634.65957446808522</v>
+      </c>
+      <c r="AE21">
+        <f t="shared" si="7"/>
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31">
       <c r="A22">
         <v>650</v>
       </c>
@@ -8012,8 +8288,24 @@
         <f t="shared" si="1"/>
         <v>687.86170212765967</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="AB22">
+        <f t="shared" si="4"/>
+        <v>650</v>
+      </c>
+      <c r="AC22">
+        <f t="shared" si="5"/>
+        <v>646.59</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="6"/>
+        <v>687.86170212765967</v>
+      </c>
+      <c r="AE22">
+        <f t="shared" si="7"/>
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31">
       <c r="A23">
         <v>700</v>
       </c>
@@ -8042,8 +8334,24 @@
         <f t="shared" si="1"/>
         <v>734.81052631578962</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="AB23">
+        <f t="shared" si="4"/>
+        <v>700</v>
+      </c>
+      <c r="AC23">
+        <f t="shared" si="5"/>
+        <v>698.07</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="6"/>
+        <v>734.81052631578962</v>
+      </c>
+      <c r="AE23">
+        <f t="shared" si="7"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31">
       <c r="A24">
         <v>750</v>
       </c>
@@ -8072,8 +8380,24 @@
         <f t="shared" si="1"/>
         <v>788.41052631578953</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="AB24">
+        <f t="shared" si="4"/>
+        <v>750</v>
+      </c>
+      <c r="AC24">
+        <f t="shared" si="5"/>
+        <v>748.99</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="6"/>
+        <v>788.41052631578953</v>
+      </c>
+      <c r="AE24">
+        <f t="shared" si="7"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31">
       <c r="A25">
         <v>800</v>
       </c>
@@ -8102,8 +8426,24 @@
         <f t="shared" si="1"/>
         <v>832.14583333333337</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="AB25">
+        <f t="shared" si="4"/>
+        <v>800</v>
+      </c>
+      <c r="AC25">
+        <f t="shared" si="5"/>
+        <v>798.86</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="6"/>
+        <v>832.14583333333337</v>
+      </c>
+      <c r="AE25">
+        <f t="shared" si="7"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31">
       <c r="A26">
         <v>850</v>
       </c>
@@ -8132,8 +8472,24 @@
         <f t="shared" si="1"/>
         <v>884.57291666666674</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="AB26">
+        <f t="shared" si="4"/>
+        <v>850</v>
+      </c>
+      <c r="AC26">
+        <f t="shared" si="5"/>
+        <v>849.19</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="6"/>
+        <v>884.57291666666674</v>
+      </c>
+      <c r="AE26">
+        <f t="shared" si="7"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31">
       <c r="A27">
         <v>900</v>
       </c>
@@ -8162,8 +8518,24 @@
         <f t="shared" si="1"/>
         <v>937.59375000000011</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="AB27">
+        <f t="shared" si="4"/>
+        <v>900</v>
+      </c>
+      <c r="AC27">
+        <f t="shared" si="5"/>
+        <v>900.09</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="6"/>
+        <v>937.59375000000011</v>
+      </c>
+      <c r="AE27">
+        <f t="shared" si="7"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31">
       <c r="A28">
         <v>950</v>
       </c>
@@ -8192,8 +8564,24 @@
         <f t="shared" si="1"/>
         <v>991.34375000000011</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="AB28">
+        <f t="shared" si="4"/>
+        <v>950</v>
+      </c>
+      <c r="AC28">
+        <f t="shared" si="5"/>
+        <v>951.69</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="6"/>
+        <v>991.34375000000011</v>
+      </c>
+      <c r="AE28">
+        <f t="shared" si="7"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31">
       <c r="A29">
         <v>1000</v>
       </c>
@@ -8222,8 +8610,24 @@
         <f t="shared" si="1"/>
         <v>1044.1666666666667</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="AB29">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="AC29">
+        <f t="shared" si="5"/>
+        <v>1002.4</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="6"/>
+        <v>1044.1666666666667</v>
+      </c>
+      <c r="AE29">
+        <f t="shared" si="7"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31">
       <c r="A30">
         <v>1050</v>
       </c>
@@ -8252,8 +8656,24 @@
         <f t="shared" si="1"/>
         <v>1090.4948453608247</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="AB30">
+        <f t="shared" si="4"/>
+        <v>1050</v>
+      </c>
+      <c r="AC30">
+        <f t="shared" si="5"/>
+        <v>1057.78</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" si="6"/>
+        <v>1090.4948453608247</v>
+      </c>
+      <c r="AE30">
+        <f t="shared" si="7"/>
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31">
       <c r="A31">
         <v>1100</v>
       </c>
@@ -8282,8 +8702,24 @@
         <f t="shared" si="1"/>
         <v>1139.0309278350514</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="AB31">
+        <f t="shared" si="4"/>
+        <v>1100</v>
+      </c>
+      <c r="AC31">
+        <f t="shared" si="5"/>
+        <v>1104.8599999999999</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="6"/>
+        <v>1139.0309278350514</v>
+      </c>
+      <c r="AE31">
+        <f t="shared" si="7"/>
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31">
       <c r="A32">
         <v>1150</v>
       </c>
@@ -8312,8 +8748,24 @@
         <f t="shared" si="1"/>
         <v>1191.3917525773197</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="AB32">
+        <f t="shared" si="4"/>
+        <v>1150</v>
+      </c>
+      <c r="AC32">
+        <f t="shared" si="5"/>
+        <v>1155.6500000000001</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="6"/>
+        <v>1191.3917525773197</v>
+      </c>
+      <c r="AE32">
+        <f t="shared" si="7"/>
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31">
       <c r="A33">
         <v>1200</v>
       </c>
@@ -8342,8 +8794,24 @@
         <f t="shared" si="1"/>
         <v>1231.6428571428571</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="AB33">
+        <f t="shared" si="4"/>
+        <v>1200</v>
+      </c>
+      <c r="AC33">
+        <f t="shared" si="5"/>
+        <v>1207.01</v>
+      </c>
+      <c r="AD33">
+        <f t="shared" si="6"/>
+        <v>1231.6428571428571</v>
+      </c>
+      <c r="AE33">
+        <f t="shared" si="7"/>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31">
       <c r="F34">
         <f>AVERAGE(F6:F33)</f>
         <v>2.392142857142848</v>
@@ -8353,7 +8821,7 @@
         <v>1.1387727317453986</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:31">
       <c r="F36" s="5" t="s">
         <v>16</v>
       </c>
@@ -8362,7 +8830,7 @@
         <v>2.3168965517241289</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:31">
       <c r="F37" s="5" t="s">
         <v>15</v>
       </c>
@@ -8371,7 +8839,7 @@
         <v>1.1387727317453986</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:31">
       <c r="F38" s="5" t="s">
         <v>17</v>
       </c>
@@ -8396,7 +8864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -8494,11 +8962,11 @@
         <v>0.98999999999998067</v>
       </c>
       <c r="K5" s="3">
-        <f>J5/I5*100</f>
+        <f t="shared" ref="K5:K19" si="0">J5/I5*100</f>
         <v>0.61047049392611508</v>
       </c>
       <c r="L5">
-        <f>F5/G5</f>
+        <f t="shared" ref="L5:L10" si="1">F5/G5</f>
         <v>255.84126984126985</v>
       </c>
     </row>
@@ -8528,19 +8996,19 @@
         <v>26.77</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I19" si="0">IF(B6&gt;0,B6,D6)</f>
+        <f t="shared" ref="I6:I19" si="2">IF(B6&gt;0,B6,D6)</f>
         <v>106.63</v>
       </c>
       <c r="J6">
-        <f t="shared" ref="J6:J19" si="1">ABS(I6-F6)</f>
+        <f t="shared" ref="J6:J19" si="3">ABS(I6-F6)</f>
         <v>36.97</v>
       </c>
       <c r="K6" s="3">
-        <f>J6/I6*100</f>
+        <f t="shared" si="0"/>
         <v>34.671293257057116</v>
       </c>
       <c r="L6">
-        <f>F6/G6</f>
+        <f t="shared" si="1"/>
         <v>287.2</v>
       </c>
     </row>
@@ -8570,19 +9038,19 @@
         <v>1.71</v>
       </c>
       <c r="I7">
+        <f t="shared" si="2"/>
+        <v>235.21</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>2.9599999999999795</v>
+      </c>
+      <c r="K7" s="3">
         <f t="shared" si="0"/>
-        <v>235.21</v>
-      </c>
-      <c r="J7">
+        <v>1.2584498958377532</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="1"/>
-        <v>2.9599999999999795</v>
-      </c>
-      <c r="K7" s="3">
-        <f>J7/I7*100</f>
-        <v>1.2584498958377532</v>
-      </c>
-      <c r="L7">
-        <f>F7/G7</f>
         <v>309.31168831168827</v>
       </c>
     </row>
@@ -8612,19 +9080,19 @@
         <v>40.06</v>
       </c>
       <c r="I8">
+        <f t="shared" si="2"/>
+        <v>51.1</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="K8" s="3">
         <f t="shared" si="0"/>
-        <v>51.1</v>
-      </c>
-      <c r="J8">
+        <v>39.921722113502931</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="1"/>
-        <v>20.399999999999999</v>
-      </c>
-      <c r="K8" s="3">
-        <f>J8/I8*100</f>
-        <v>39.921722113502931</v>
-      </c>
-      <c r="L8">
-        <f>F8/G8</f>
         <v>255.35714285714283</v>
       </c>
     </row>
@@ -8654,19 +9122,19 @@
         <v>69.489999999999995</v>
       </c>
       <c r="I9">
+        <f t="shared" si="2"/>
+        <v>305.54000000000002</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>1.9300000000000068</v>
+      </c>
+      <c r="K9" s="3">
         <f t="shared" si="0"/>
-        <v>305.54000000000002</v>
-      </c>
-      <c r="J9">
+        <v>0.63166852130654139</v>
+      </c>
+      <c r="L9">
         <f t="shared" si="1"/>
-        <v>1.9300000000000068</v>
-      </c>
-      <c r="K9" s="3">
-        <f>J9/I9*100</f>
-        <v>0.63166852130654139</v>
-      </c>
-      <c r="L9">
-        <f>F9/G9</f>
         <v>394.2987012987013</v>
       </c>
     </row>
@@ -8696,19 +9164,19 @@
         <v>17.329999999999998</v>
       </c>
       <c r="I10">
+        <f t="shared" si="2"/>
+        <v>48.57</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>9.509999999999998</v>
+      </c>
+      <c r="K10" s="3">
         <f t="shared" si="0"/>
-        <v>48.57</v>
-      </c>
-      <c r="J10">
+        <v>19.579987646695489</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="1"/>
-        <v>9.509999999999998</v>
-      </c>
-      <c r="K10" s="3">
-        <f>J10/I10*100</f>
-        <v>19.579987646695489</v>
-      </c>
-      <c r="L10">
-        <f>F10/G10</f>
         <v>205.57894736842107</v>
       </c>
     </row>
@@ -8732,19 +9200,19 @@
         <v>8.07</v>
       </c>
       <c r="I11">
+        <f t="shared" si="2"/>
+        <v>108.22</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>5.2999999999999972</v>
+      </c>
+      <c r="K11" s="3">
         <f t="shared" si="0"/>
-        <v>108.22</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="1"/>
-        <v>5.2999999999999972</v>
-      </c>
-      <c r="K11" s="3">
-        <f>J11/I11*100</f>
         <v>4.89743115875069</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11:L19" si="2">F11/G11</f>
+        <f t="shared" ref="L11:L19" si="4">F11/G11</f>
         <v>233.90909090909091</v>
       </c>
     </row>
@@ -8774,19 +9242,19 @@
         <v>152.66999999999999</v>
       </c>
       <c r="I12">
+        <f t="shared" si="2"/>
+        <v>196.23</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>9.0300000000000011</v>
+      </c>
+      <c r="K12" s="3">
         <f t="shared" si="0"/>
-        <v>196.23</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="1"/>
-        <v>9.0300000000000011</v>
-      </c>
-      <c r="K12" s="3">
-        <f>J12/I12*100</f>
         <v>4.6017428527748061</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>390</v>
       </c>
     </row>
@@ -8816,19 +9284,19 @@
         <v>24.11</v>
       </c>
       <c r="I13">
+        <f t="shared" si="2"/>
+        <v>129.51</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>3.9999999999999858</v>
+      </c>
+      <c r="K13" s="3">
         <f t="shared" si="0"/>
-        <v>129.51</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="1"/>
-        <v>3.9999999999999858</v>
-      </c>
-      <c r="K13" s="3">
-        <f>J13/I13*100</f>
         <v>3.0885645896069693</v>
       </c>
       <c r="L13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>278.9111111111111</v>
       </c>
     </row>
@@ -8858,19 +9326,19 @@
         <v>10.46</v>
       </c>
       <c r="I14">
+        <f t="shared" si="2"/>
+        <v>50.44</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>0.82999999999999829</v>
+      </c>
+      <c r="K14" s="3">
         <f t="shared" si="0"/>
-        <v>50.44</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="1"/>
-        <v>0.82999999999999829</v>
-      </c>
-      <c r="K14" s="3">
-        <f>J14/I14*100</f>
         <v>1.6455194290245803</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>225.5</v>
       </c>
     </row>
@@ -8900,19 +9368,19 @@
         <v>2.31</v>
       </c>
       <c r="I15">
+        <f t="shared" si="2"/>
+        <v>9.11</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>0.61999999999999922</v>
+      </c>
+      <c r="K15" s="3">
         <f t="shared" si="0"/>
-        <v>9.11</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="1"/>
-        <v>0.61999999999999922</v>
-      </c>
-      <c r="K15" s="3">
-        <f>J15/I15*100</f>
         <v>6.8057080131723309</v>
       </c>
       <c r="L15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>141.5</v>
       </c>
     </row>
@@ -8936,19 +9404,19 @@
         <v>238.36</v>
       </c>
       <c r="I16">
+        <f t="shared" si="2"/>
+        <v>1729.73</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>16.009999999999991</v>
+      </c>
+      <c r="K16" s="3">
         <f t="shared" si="0"/>
-        <v>1729.73</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="1"/>
-        <v>16.009999999999991</v>
-      </c>
-      <c r="K16" s="3">
-        <f>J16/I16*100</f>
         <v>0.92557798037844008</v>
       </c>
       <c r="L16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1918.3956043956043</v>
       </c>
     </row>
@@ -8972,19 +9440,19 @@
         <v>12.09</v>
       </c>
       <c r="I17">
+        <f t="shared" si="2"/>
+        <v>827.87</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>22.110000000000014</v>
+      </c>
+      <c r="K17" s="3">
         <f t="shared" si="0"/>
-        <v>827.87</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="1"/>
-        <v>22.110000000000014</v>
-      </c>
-      <c r="K17" s="3">
-        <f>J17/I17*100</f>
         <v>2.6707091693140246</v>
       </c>
       <c r="L17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>839.33333333333337</v>
       </c>
     </row>
@@ -9008,19 +9476,19 @@
         <v>24.57</v>
       </c>
       <c r="I18">
+        <f t="shared" si="2"/>
+        <v>1246.96</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>15.240000000000009</v>
+      </c>
+      <c r="K18" s="3">
         <f t="shared" si="0"/>
-        <v>1246.96</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="1"/>
-        <v>15.240000000000009</v>
-      </c>
-      <c r="K18" s="3">
-        <f>J18/I18*100</f>
         <v>1.222172323089755</v>
       </c>
       <c r="L18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1287.9591836734694</v>
       </c>
     </row>
@@ -9050,19 +9518,19 @@
         <v>4.91</v>
       </c>
       <c r="I19">
+        <f t="shared" si="2"/>
+        <v>52.68</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>4.490000000000002</v>
+      </c>
+      <c r="K19" s="3">
         <f t="shared" si="0"/>
-        <v>52.68</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="1"/>
-        <v>4.490000000000002</v>
-      </c>
-      <c r="K19" s="3">
-        <f>J19/I19*100</f>
         <v>8.5231586940015234</v>
       </c>
       <c r="L19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>192.76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added stdev to calib and measure
</commit_message>
<xml_diff>
--- a/software/ble/Calib_and_Measure.xlsx
+++ b/software/ble/Calib_and_Measure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22160" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
   <si>
     <t>Power</t>
   </si>
@@ -135,6 +135,12 @@
   <si>
     <t>Microwave</t>
   </si>
+  <si>
+    <t>Stddev:</t>
+  </si>
+  <si>
+    <t>Average:</t>
+  </si>
 </sst>
 </file>
 
@@ -190,8 +196,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -209,11 +217,13 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -480,11 +490,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123876680"/>
-        <c:axId val="2123873784"/>
+        <c:axId val="2141612856"/>
+        <c:axId val="2141615784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123876680"/>
+        <c:axId val="2141612856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,12 +504,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123873784"/>
+        <c:crossAx val="2141615784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123873784"/>
+        <c:axId val="2141615784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,7 +520,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123876680"/>
+        <c:crossAx val="2141612856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -576,64 +586,64 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>'Measurement - new non unity'!$F$5:$F$33</c:f>
+              <c:f>'Measurement - new non unity'!$D$5:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>161.18</c:v>
+                  <c:v>163.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>143.6</c:v>
+                  <c:v>108.58</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>238.17</c:v>
+                  <c:v>236.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>71.5</c:v>
+                  <c:v>55.28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>303.61</c:v>
+                  <c:v>306.42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39.06</c:v>
+                  <c:v>47.49</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>102.92</c:v>
+                  <c:v>108.22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>187.2</c:v>
+                  <c:v>197.09</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>125.51</c:v>
+                  <c:v>129.47</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>49.61</c:v>
+                  <c:v>51.08</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.49</c:v>
+                  <c:v>9.33</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1745.74</c:v>
+                  <c:v>1729.73</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>805.76</c:v>
+                  <c:v>827.87</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1262.2</c:v>
+                  <c:v>1246.96</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>48.19</c:v>
+                  <c:v>52.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Measurement - new non unity'!$J$5:$J$33</c:f>
+              <c:f>'Measurement - new non unity'!$J$5:$J$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0.989999999999981</c:v>
                 </c:pt>
@@ -678,15 +688,6 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>4.490000000000002</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -701,11 +702,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123466088"/>
-        <c:axId val="2123463128"/>
+        <c:axId val="2053272696"/>
+        <c:axId val="2053269736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123466088"/>
+        <c:axId val="2053272696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -715,12 +716,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123463128"/>
+        <c:crossAx val="2053269736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123463128"/>
+        <c:axId val="2053269736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -731,7 +732,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123466088"/>
+        <c:crossAx val="2053272696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -797,64 +798,65 @@
             </a:ln>
           </c:spPr>
           <c:xVal>
-            <c:strRef>
-              <c:f>'Measurement - new non unity'!$A$5:$A$33</c:f>
-              <c:strCache>
+            <c:numRef>
+              <c:f>'Measurement - new non unity'!$D$5:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>150 W Bulb</c:v>
+                  <c:v>163.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Blender</c:v>
+                  <c:v>108.58</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Drill max</c:v>
+                  <c:v>236.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Drill low</c:v>
+                  <c:v>55.28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Hot Air</c:v>
+                  <c:v>306.42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50W CFL</c:v>
+                  <c:v>47.49</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Fridge</c:v>
+                  <c:v>108.22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Tv full</c:v>
+                  <c:v>197.09</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>TV low</c:v>
+                  <c:v>129.47</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Xbox</c:v>
+                  <c:v>51.08</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Router</c:v>
+                  <c:v>9.33</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Microwave</c:v>
+                  <c:v>1729.73</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Toaster</c:v>
+                  <c:v>827.87</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Vacuum</c:v>
+                  <c:v>1246.96</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>MacBook</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>52.27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Measurement - new non unity'!$K$5:$K$33</c:f>
+              <c:f>'Measurement - new non unity'!$K$5:$K$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0.610470493926115</c:v>
                 </c:pt>
@@ -899,15 +901,6 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>8.523158694001523</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>10.026</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>8.736945075895937</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>11.16323606915134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -922,11 +915,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123436120"/>
-        <c:axId val="2123433160"/>
+        <c:axId val="2053242728"/>
+        <c:axId val="2053239768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123436120"/>
+        <c:axId val="2053242728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,12 +929,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123433160"/>
+        <c:crossAx val="2053239768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123433160"/>
+        <c:axId val="2053239768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22.0"/>
@@ -953,7 +946,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123436120"/>
+        <c:crossAx val="2053242728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1342,8 +1335,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123791752"/>
-        <c:axId val="2123788760"/>
+        <c:axId val="2141708664"/>
+        <c:axId val="2141711656"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1521,11 +1514,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123782488"/>
-        <c:axId val="2123785432"/>
+        <c:axId val="2141717928"/>
+        <c:axId val="2141714984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123791752"/>
+        <c:axId val="2141708664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1535,12 +1528,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123788760"/>
+        <c:crossAx val="2141711656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123788760"/>
+        <c:axId val="2141711656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600.0"/>
@@ -1553,12 +1546,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123791752"/>
+        <c:crossAx val="2141708664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123785432"/>
+        <c:axId val="2141714984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1570,12 +1563,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123782488"/>
+        <c:crossAx val="2141717928"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123782488"/>
+        <c:axId val="2141717928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1585,7 +1578,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123785432"/>
+        <c:crossAx val="2141714984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2084,8 +2077,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123733528"/>
-        <c:axId val="2123730968"/>
+        <c:axId val="2141764280"/>
+        <c:axId val="2141769672"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2323,11 +2316,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123724696"/>
-        <c:axId val="2123727640"/>
+        <c:axId val="2141775944"/>
+        <c:axId val="2141773000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123733528"/>
+        <c:axId val="2141764280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2337,12 +2330,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123730968"/>
+        <c:crossAx val="2141769672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123730968"/>
+        <c:axId val="2141769672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2353,12 +2346,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123733528"/>
+        <c:crossAx val="2141764280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123727640"/>
+        <c:axId val="2141773000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -2370,12 +2363,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123724696"/>
+        <c:crossAx val="2141775944"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123724696"/>
+        <c:axId val="2141775944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2385,7 +2378,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123727640"/>
+        <c:crossAx val="2141773000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2650,11 +2643,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123704440"/>
-        <c:axId val="2123701480"/>
+        <c:axId val="2141796184"/>
+        <c:axId val="2141799144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123704440"/>
+        <c:axId val="2141796184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2664,12 +2657,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123701480"/>
+        <c:crossAx val="2141799144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123701480"/>
+        <c:axId val="2141799144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50.0"/>
@@ -2681,7 +2674,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123704440"/>
+        <c:crossAx val="2141796184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2946,11 +2939,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123674984"/>
-        <c:axId val="2123672024"/>
+        <c:axId val="2053996856"/>
+        <c:axId val="2053999816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123674984"/>
+        <c:axId val="2053996856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2960,12 +2953,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123672024"/>
+        <c:crossAx val="2053999816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123672024"/>
+        <c:axId val="2053999816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22.0"/>
@@ -2977,7 +2970,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123674984"/>
+        <c:crossAx val="2053996856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3476,8 +3469,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123617688"/>
-        <c:axId val="2123615128"/>
+        <c:axId val="2054059912"/>
+        <c:axId val="2054065304"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3715,11 +3708,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123608856"/>
-        <c:axId val="2123611800"/>
+        <c:axId val="2054071576"/>
+        <c:axId val="2054068632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123617688"/>
+        <c:axId val="2054059912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3729,12 +3722,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123615128"/>
+        <c:crossAx val="2054065304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123615128"/>
+        <c:axId val="2054065304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3745,12 +3738,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123617688"/>
+        <c:crossAx val="2054059912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123611800"/>
+        <c:axId val="2054068632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -3762,12 +3755,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123608856"/>
+        <c:crossAx val="2054071576"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123608856"/>
+        <c:axId val="2054071576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3777,7 +3770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123611800"/>
+        <c:crossAx val="2054068632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4044,11 +4037,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123586744"/>
-        <c:axId val="2123583784"/>
+        <c:axId val="2054092776"/>
+        <c:axId val="2054095736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123586744"/>
+        <c:axId val="2054092776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4058,12 +4051,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123583784"/>
+        <c:crossAx val="2054095736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123583784"/>
+        <c:axId val="2054095736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4074,7 +4067,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123586744"/>
+        <c:crossAx val="2054092776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4341,11 +4334,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123556376"/>
-        <c:axId val="2123553416"/>
+        <c:axId val="2054123704"/>
+        <c:axId val="2054126664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123556376"/>
+        <c:axId val="2054123704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4355,12 +4348,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123553416"/>
+        <c:crossAx val="2054126664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123553416"/>
+        <c:axId val="2054126664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22.0"/>
@@ -4372,7 +4365,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123556376"/>
+        <c:crossAx val="2054123704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4447,52 +4440,64 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Measurement - new non unity'!$B$5:$B$33</c:f>
+              <c:f>'Measurement - new non unity'!$D$5:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>162.17</c:v>
+                  <c:v>163.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>106.63</c:v>
+                  <c:v>108.58</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>235.21</c:v>
+                  <c:v>236.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51.1</c:v>
+                  <c:v>55.28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>305.54</c:v>
+                  <c:v>306.42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.57</c:v>
+                  <c:v>47.49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>108.22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>196.23</c:v>
+                  <c:v>197.09</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>129.51</c:v>
+                  <c:v>129.47</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50.44</c:v>
+                  <c:v>51.08</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.11</c:v>
+                  <c:v>9.33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1729.73</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>827.87</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1246.96</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>52.68</c:v>
+                  <c:v>52.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Measurement - new non unity'!$F$5:$F$33</c:f>
+              <c:f>'Measurement - new non unity'!$F$5:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>161.18</c:v>
                 </c:pt>
@@ -4576,52 +4581,64 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Measurement - new non unity'!$B$5:$B$33</c:f>
+              <c:f>'Measurement - new non unity'!$D$5:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>162.17</c:v>
+                  <c:v>163.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>106.63</c:v>
+                  <c:v>108.58</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>235.21</c:v>
+                  <c:v>236.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51.1</c:v>
+                  <c:v>55.28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>305.54</c:v>
+                  <c:v>306.42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.57</c:v>
+                  <c:v>47.49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>108.22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>196.23</c:v>
+                  <c:v>197.09</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>129.51</c:v>
+                  <c:v>129.47</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50.44</c:v>
+                  <c:v>51.08</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.11</c:v>
+                  <c:v>9.33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1729.73</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>827.87</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1246.96</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>52.68</c:v>
+                  <c:v>52.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Measurement - new non unity'!$B$5:$B$33</c:f>
+              <c:f>'Measurement - new non unity'!$B$5:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>162.17</c:v>
                 </c:pt>
@@ -4668,8 +4685,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123496008"/>
-        <c:axId val="2123493448"/>
+        <c:axId val="2053302616"/>
+        <c:axId val="2053300056"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4707,52 +4724,64 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Measurement - new non unity'!$B$5:$B$33</c:f>
+              <c:f>'Measurement - new non unity'!$D$5:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>162.17</c:v>
+                  <c:v>163.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>106.63</c:v>
+                  <c:v>108.58</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>235.21</c:v>
+                  <c:v>236.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51.1</c:v>
+                  <c:v>55.28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>305.54</c:v>
+                  <c:v>306.42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.57</c:v>
+                  <c:v>47.49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>108.22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>196.23</c:v>
+                  <c:v>197.09</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>129.51</c:v>
+                  <c:v>129.47</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50.44</c:v>
+                  <c:v>51.08</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.11</c:v>
+                  <c:v>9.33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1729.73</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>827.87</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1246.96</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>52.68</c:v>
+                  <c:v>52.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Measurement - new non unity'!$G$5:$G$33</c:f>
+              <c:f>'Measurement - new non unity'!$G$5:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0.63</c:v>
                 </c:pt>
@@ -4811,11 +4840,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123487176"/>
-        <c:axId val="2123490120"/>
+        <c:axId val="2053293784"/>
+        <c:axId val="2053296728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123496008"/>
+        <c:axId val="2053302616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4825,12 +4854,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123493448"/>
+        <c:crossAx val="2053300056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123493448"/>
+        <c:axId val="2053300056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4841,12 +4870,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123496008"/>
+        <c:crossAx val="2053302616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123490120"/>
+        <c:axId val="2053296728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -4858,12 +4887,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123487176"/>
+        <c:crossAx val="2053293784"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123487176"/>
+        <c:axId val="2053293784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4873,7 +4902,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123490120"/>
+        <c:crossAx val="2053296728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7420,13 +7449,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE38"/>
+  <dimension ref="A1:AE44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE33" sqref="AB5:AE33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E40" sqref="E40:J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="9" max="9" width="8.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" t="s">
@@ -7502,6 +7534,14 @@
         <f t="shared" ref="H5:H33" si="1">C5/D5</f>
         <v>60.25</v>
       </c>
+      <c r="I5">
+        <f>IF(F5&gt;(F$40+F$41),"",F5)</f>
+        <v>0.20999999999999996</v>
+      </c>
+      <c r="J5" t="str">
+        <f>IF(G5&gt;(G$43+G$44),"",G5)</f>
+        <v/>
+      </c>
       <c r="AB5">
         <f>B5</f>
         <v>2.2000000000000002</v>
@@ -7548,20 +7588,28 @@
         <f t="shared" si="1"/>
         <v>99.199999999999989</v>
       </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I33" si="4">IF(F6&gt;(F$40+F$41),"",F6)</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J33" si="5">IF(G6&gt;(G$43+G$44),"",G6)</f>
+        <v>0.80000000000000071</v>
+      </c>
       <c r="AB6">
-        <f t="shared" ref="AB6:AB38" si="4">B6</f>
+        <f t="shared" ref="AB6:AB33" si="6">B6</f>
         <v>5</v>
       </c>
       <c r="AC6">
-        <f t="shared" ref="AC6:AC38" si="5">C6</f>
+        <f t="shared" ref="AC6:AC33" si="7">C6</f>
         <v>4.96</v>
       </c>
       <c r="AD6">
-        <f t="shared" ref="AD6:AD38" si="6">H6</f>
+        <f t="shared" ref="AD6:AD33" si="8">H6</f>
         <v>99.199999999999989</v>
       </c>
       <c r="AE6">
-        <f t="shared" ref="AE6:AE38" si="7">D6</f>
+        <f t="shared" ref="AE6:AE33" si="9">D6</f>
         <v>0.05</v>
       </c>
     </row>
@@ -7594,20 +7642,28 @@
         <f t="shared" si="1"/>
         <v>155.00000000000003</v>
       </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>0.69999999999999929</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="AB7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.3000000000000007</v>
       </c>
       <c r="AD7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>155.00000000000003</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.06</v>
       </c>
     </row>
@@ -7640,20 +7696,28 @@
         <f t="shared" si="1"/>
         <v>184.5625</v>
       </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>0.46999999999999886</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="5"/>
+        <v>1.5666666666666627</v>
+      </c>
       <c r="AB8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>29.53</v>
       </c>
       <c r="AD8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>184.5625</v>
       </c>
       <c r="AE8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.16</v>
       </c>
     </row>
@@ -7686,20 +7750,28 @@
         <f t="shared" si="1"/>
         <v>202.92</v>
       </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>0.72999999999999687</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="5"/>
+        <v>1.4599999999999937</v>
+      </c>
       <c r="AB9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>50.73</v>
       </c>
       <c r="AD9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>202.92</v>
       </c>
       <c r="AE9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.25</v>
       </c>
     </row>
@@ -7732,20 +7804,28 @@
         <f t="shared" si="1"/>
         <v>211.94444444444446</v>
       </c>
+      <c r="I10">
+        <f t="shared" si="4"/>
+        <v>1.0999999999999943</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="5"/>
+        <v>1.4627659574468008</v>
+      </c>
       <c r="AB10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>75.2</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>76.3</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>211.94444444444446</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.36</v>
       </c>
     </row>
@@ -7778,20 +7858,28 @@
         <f t="shared" si="1"/>
         <v>224.53333333333333</v>
       </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>1.0400000000000063</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="5"/>
+        <v>1.0400000000000063</v>
+      </c>
       <c r="AB11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>101.04</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>224.53333333333333</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.45</v>
       </c>
     </row>
@@ -7824,20 +7912,28 @@
         <f t="shared" si="1"/>
         <v>254.35593220338984</v>
       </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>6.9999999999993179E-2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="5"/>
+        <v>4.6666666666662117E-2</v>
+      </c>
       <c r="AB12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>150.07</v>
       </c>
       <c r="AD12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>254.35593220338984</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.59</v>
       </c>
     </row>
@@ -7870,20 +7966,28 @@
         <f t="shared" si="1"/>
         <v>284.85714285714289</v>
       </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
+        <v>0.59999999999999432</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="5"/>
+        <v>0.29999999999999716</v>
+      </c>
       <c r="AB13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>199.4</v>
       </c>
       <c r="AD13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>284.85714285714289</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.7</v>
       </c>
     </row>
@@ -7916,20 +8020,28 @@
         <f t="shared" si="1"/>
         <v>317.84615384615381</v>
       </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
+        <v>2.0800000000000125</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="5"/>
+        <v>0.83200000000000496</v>
+      </c>
       <c r="AB14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>250</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>247.92</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>317.84615384615381</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.78</v>
       </c>
     </row>
@@ -7962,20 +8074,28 @@
         <f t="shared" si="1"/>
         <v>358.09638554216872</v>
       </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>2.7799999999999727</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="5"/>
+        <v>0.92666666666665765</v>
+      </c>
       <c r="AB15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>297.22000000000003</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>358.09638554216872</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.83</v>
       </c>
     </row>
@@ -8008,20 +8128,28 @@
         <f t="shared" si="1"/>
         <v>403.76744186046511</v>
       </c>
+      <c r="I16">
+        <f t="shared" si="4"/>
+        <v>2.7599999999999909</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="5"/>
+        <v>0.78857142857142604</v>
+      </c>
       <c r="AB16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>350</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>347.24</v>
       </c>
       <c r="AD16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>403.76744186046511</v>
       </c>
       <c r="AE16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.86</v>
       </c>
     </row>
@@ -8054,20 +8182,28 @@
         <f t="shared" si="1"/>
         <v>445.8089887640449</v>
       </c>
+      <c r="I17">
+        <f t="shared" si="4"/>
+        <v>3.2300000000000182</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="5"/>
+        <v>0.80750000000000455</v>
+      </c>
       <c r="AB17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>400</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>396.77</v>
       </c>
       <c r="AD17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>445.8089887640449</v>
       </c>
       <c r="AE17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.89</v>
       </c>
     </row>
@@ -8100,20 +8236,28 @@
         <f t="shared" si="1"/>
         <v>496.4111111111111</v>
       </c>
+      <c r="I18">
+        <f t="shared" si="4"/>
+        <v>2.2300000000000182</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="5"/>
+        <v>0.49665924276169665</v>
+      </c>
       <c r="AB18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>449</v>
       </c>
       <c r="AC18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>446.77</v>
       </c>
       <c r="AD18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>496.4111111111111</v>
       </c>
       <c r="AE18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.9</v>
       </c>
     </row>
@@ -8147,23 +8291,27 @@
         <v>538.46739130434776</v>
       </c>
       <c r="I19">
-        <f>AVERAGE(G6:G19)</f>
-        <v>1.3107371036859092</v>
+        <f t="shared" si="4"/>
+        <v>4.1100000000000136</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
+        <v>0.82282282282282559</v>
       </c>
       <c r="AB19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>499.5</v>
       </c>
       <c r="AC19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>495.39</v>
       </c>
       <c r="AD19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>538.46739130434776</v>
       </c>
       <c r="AE19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.92</v>
       </c>
     </row>
@@ -8196,20 +8344,28 @@
         <f t="shared" si="1"/>
         <v>585.97849462365593</v>
       </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>3.8399999999999181</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="5"/>
+        <v>0.69970845481048083</v>
+      </c>
       <c r="AB20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>548.79999999999995</v>
       </c>
       <c r="AC20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>544.96</v>
       </c>
       <c r="AD20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>585.97849462365593</v>
       </c>
       <c r="AE20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.93</v>
       </c>
     </row>
@@ -8242,20 +8398,28 @@
         <f t="shared" si="1"/>
         <v>634.65957446808522</v>
       </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>3.4199999999999591</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="5"/>
+        <v>0.56999999999999318</v>
+      </c>
       <c r="AB21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>600</v>
       </c>
       <c r="AC21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>596.58000000000004</v>
       </c>
       <c r="AD21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>634.65957446808522</v>
       </c>
       <c r="AE21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.94</v>
       </c>
     </row>
@@ -8288,20 +8452,28 @@
         <f t="shared" si="1"/>
         <v>687.86170212765967</v>
       </c>
+      <c r="I22">
+        <f t="shared" si="4"/>
+        <v>3.4099999999999682</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="5"/>
+        <v>0.52461538461537971</v>
+      </c>
       <c r="AB22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>650</v>
       </c>
       <c r="AC22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>646.59</v>
       </c>
       <c r="AD22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>687.86170212765967</v>
       </c>
       <c r="AE22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.94</v>
       </c>
     </row>
@@ -8334,20 +8506,28 @@
         <f t="shared" si="1"/>
         <v>734.81052631578962</v>
       </c>
+      <c r="I23">
+        <f t="shared" si="4"/>
+        <v>1.92999999999995</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="5"/>
+        <v>0.27571428571427858</v>
+      </c>
       <c r="AB23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>700</v>
       </c>
       <c r="AC23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>698.07</v>
       </c>
       <c r="AD23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>734.81052631578962</v>
       </c>
       <c r="AE23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.95</v>
       </c>
     </row>
@@ -8380,20 +8560,28 @@
         <f t="shared" si="1"/>
         <v>788.41052631578953</v>
       </c>
+      <c r="I24">
+        <f t="shared" si="4"/>
+        <v>1.0099999999999909</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="5"/>
+        <v>0.13466666666666544</v>
+      </c>
       <c r="AB24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>750</v>
       </c>
       <c r="AC24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>748.99</v>
       </c>
       <c r="AD24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>788.41052631578953</v>
       </c>
       <c r="AE24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.95</v>
       </c>
     </row>
@@ -8426,20 +8614,28 @@
         <f t="shared" si="1"/>
         <v>832.14583333333337</v>
       </c>
+      <c r="I25">
+        <f t="shared" si="4"/>
+        <v>1.1399999999999864</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="5"/>
+        <v>0.14249999999999829</v>
+      </c>
       <c r="AB25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>800</v>
       </c>
       <c r="AC25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>798.86</v>
       </c>
       <c r="AD25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>832.14583333333337</v>
       </c>
       <c r="AE25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.96</v>
       </c>
     </row>
@@ -8472,20 +8668,28 @@
         <f t="shared" si="1"/>
         <v>884.57291666666674</v>
       </c>
+      <c r="I26">
+        <f t="shared" si="4"/>
+        <v>0.80999999999994543</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="5"/>
+        <v>9.5294117647052409E-2</v>
+      </c>
       <c r="AB26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>850</v>
       </c>
       <c r="AC26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>849.19</v>
       </c>
       <c r="AD26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>884.57291666666674</v>
       </c>
       <c r="AE26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.96</v>
       </c>
     </row>
@@ -8518,20 +8722,28 @@
         <f t="shared" si="1"/>
         <v>937.59375000000011</v>
       </c>
+      <c r="I27">
+        <f t="shared" si="4"/>
+        <v>9.0000000000031832E-2</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="5"/>
+        <v>1.0000000000003536E-2</v>
+      </c>
       <c r="AB27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>900</v>
       </c>
       <c r="AC27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>900.09</v>
       </c>
       <c r="AD27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>937.59375000000011</v>
       </c>
       <c r="AE27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.96</v>
       </c>
     </row>
@@ -8564,20 +8776,28 @@
         <f t="shared" si="1"/>
         <v>991.34375000000011</v>
       </c>
+      <c r="I28">
+        <f t="shared" si="4"/>
+        <v>1.6900000000000546</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="5"/>
+        <v>0.17789473684211102</v>
+      </c>
       <c r="AB28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>950</v>
       </c>
       <c r="AC28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>951.69</v>
       </c>
       <c r="AD28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>991.34375000000011</v>
       </c>
       <c r="AE28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.96</v>
       </c>
     </row>
@@ -8610,20 +8830,28 @@
         <f t="shared" si="1"/>
         <v>1044.1666666666667</v>
       </c>
+      <c r="I29">
+        <f t="shared" si="4"/>
+        <v>2.3999999999999773</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="5"/>
+        <v>0.23999999999999772</v>
+      </c>
       <c r="AB29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
       <c r="AC29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1002.4</v>
       </c>
       <c r="AD29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1044.1666666666667</v>
       </c>
       <c r="AE29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.96</v>
       </c>
     </row>
@@ -8656,20 +8884,28 @@
         <f t="shared" si="1"/>
         <v>1090.4948453608247</v>
       </c>
+      <c r="I30" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="J30">
+        <f t="shared" si="5"/>
+        <v>0.74095238095237836</v>
+      </c>
       <c r="AB30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1050</v>
       </c>
       <c r="AC30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1057.78</v>
       </c>
       <c r="AD30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1090.4948453608247</v>
       </c>
       <c r="AE30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.97</v>
       </c>
     </row>
@@ -8702,20 +8938,28 @@
         <f t="shared" si="1"/>
         <v>1139.0309278350514</v>
       </c>
+      <c r="I31" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="J31">
+        <f t="shared" si="5"/>
+        <v>0.44181818181817273</v>
+      </c>
       <c r="AB31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1100</v>
       </c>
       <c r="AC31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1104.8599999999999</v>
       </c>
       <c r="AD31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1139.0309278350514</v>
       </c>
       <c r="AE31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.97</v>
       </c>
     </row>
@@ -8748,20 +8992,28 @@
         <f t="shared" si="1"/>
         <v>1191.3917525773197</v>
       </c>
+      <c r="I32" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="J32">
+        <f t="shared" si="5"/>
+        <v>0.49130434782609489</v>
+      </c>
       <c r="AB32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1150</v>
       </c>
       <c r="AC32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1155.6500000000001</v>
       </c>
       <c r="AD32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1191.3917525773197</v>
       </c>
       <c r="AE32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.97</v>
       </c>
     </row>
@@ -8794,20 +9046,28 @@
         <f t="shared" si="1"/>
         <v>1231.6428571428571</v>
       </c>
+      <c r="I33" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="J33">
+        <f t="shared" si="5"/>
+        <v>0.58416666666666595</v>
+      </c>
       <c r="AB33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1200</v>
       </c>
       <c r="AC33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1207.01</v>
       </c>
       <c r="AD33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1231.6428571428571</v>
       </c>
       <c r="AE33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.98</v>
       </c>
     </row>
@@ -8846,6 +9106,70 @@
       <c r="G38">
         <f>100*SUM(F5:F33)/SUM(B5:B33)</f>
         <v>0.44438712408314807</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31">
+      <c r="E40" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40">
+        <f>AVERAGE(F5:F33)</f>
+        <v>2.3168965517241289</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I40">
+        <f>AVERAGE(I5:I29)</f>
+        <v>1.6755999999999915</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31">
+      <c r="E41" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F41">
+        <f>STDEV(F5:F33)</f>
+        <v>2.0602498174602046</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I41">
+        <f>STDEV(I5:I33)</f>
+        <v>1.276721321719549</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31">
+      <c r="F43" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43">
+        <f>AVERAGE(G5:G33)</f>
+        <v>1.1387727317453986</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J43">
+        <f>AVERAGE(J5:J33)</f>
+        <v>0.61033165463563011</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31">
+      <c r="F44" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G44">
+        <f>STDEV(G5:G33)</f>
+        <v>2.0478725995976363</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J44">
+        <f>STDEV(J5:J33)</f>
+        <v>0.43234013082033707</v>
       </c>
     </row>
   </sheetData>
@@ -8862,20 +9186,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AG34" sqref="AG34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -8890,7 +9214,7 @@
         <v>5.7459000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -8928,7 +9252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -8969,8 +9293,16 @@
         <f t="shared" ref="L5:L10" si="1">F5/G5</f>
         <v>255.84126984126985</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <f>IF(J5&gt;(J$27+J$28),"",J5)</f>
+        <v>0.98999999999998067</v>
+      </c>
+      <c r="N5">
+        <f>IF(K5&gt;(K$30+K$31),"",K5)</f>
+        <v>0.61047049392611508</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -9011,8 +9343,16 @@
         <f t="shared" si="1"/>
         <v>287.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" t="str">
+        <f t="shared" ref="M6:M19" si="4">IF(J6&gt;(J$27+J$28),"",J6)</f>
+        <v/>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" ref="N6:N19" si="5">IF(K6&gt;(K$30+K$31),"",K6)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -9053,8 +9393,16 @@
         <f t="shared" si="1"/>
         <v>309.31168831168827</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>2.9599999999999795</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="5"/>
+        <v>1.2584498958377532</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -9095,8 +9443,16 @@
         <f t="shared" si="1"/>
         <v>255.35714285714283</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -9137,8 +9493,16 @@
         <f t="shared" si="1"/>
         <v>394.2987012987013</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>1.9300000000000068</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="5"/>
+        <v>0.63166852130654139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -9179,8 +9543,16 @@
         <f t="shared" si="1"/>
         <v>205.57894736842107</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10">
+        <f t="shared" si="4"/>
+        <v>9.509999999999998</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="5"/>
+        <v>19.579987646695489</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -9212,11 +9584,19 @@
         <v>4.89743115875069</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11:L19" si="4">F11/G11</f>
+        <f t="shared" ref="L11:L19" si="6">F11/G11</f>
         <v>233.90909090909091</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11">
+        <f t="shared" si="4"/>
+        <v>5.2999999999999972</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="5"/>
+        <v>4.89743115875069</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -9254,11 +9634,19 @@
         <v>4.6017428527748061</v>
       </c>
       <c r="L12">
+        <f t="shared" si="6"/>
+        <v>390</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="4"/>
-        <v>390</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>9.0300000000000011</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="5"/>
+        <v>4.6017428527748061</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -9296,11 +9684,19 @@
         <v>3.0885645896069693</v>
       </c>
       <c r="L13">
+        <f t="shared" si="6"/>
+        <v>278.9111111111111</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="4"/>
-        <v>278.9111111111111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>3.9999999999999858</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="5"/>
+        <v>3.0885645896069693</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -9338,11 +9734,19 @@
         <v>1.6455194290245803</v>
       </c>
       <c r="L14">
+        <f t="shared" si="6"/>
+        <v>225.5</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="4"/>
-        <v>225.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>0.82999999999999829</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="5"/>
+        <v>1.6455194290245803</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -9380,11 +9784,19 @@
         <v>6.8057080131723309</v>
       </c>
       <c r="L15">
+        <f t="shared" si="6"/>
+        <v>141.5</v>
+      </c>
+      <c r="M15">
         <f t="shared" si="4"/>
-        <v>141.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>0.61999999999999922</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="5"/>
+        <v>6.8057080131723309</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -9416,11 +9828,19 @@
         <v>0.92557798037844008</v>
       </c>
       <c r="L16">
+        <f t="shared" si="6"/>
+        <v>1918.3956043956043</v>
+      </c>
+      <c r="M16">
         <f t="shared" si="4"/>
-        <v>1918.3956043956043</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>16.009999999999991</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="5"/>
+        <v>0.92557798037844008</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -9452,11 +9872,19 @@
         <v>2.6707091693140246</v>
       </c>
       <c r="L17">
+        <f t="shared" si="6"/>
+        <v>839.33333333333337</v>
+      </c>
+      <c r="M17" t="str">
         <f t="shared" si="4"/>
-        <v>839.33333333333337</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v/>
+      </c>
+      <c r="N17">
+        <f t="shared" si="5"/>
+        <v>2.6707091693140246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -9488,11 +9916,19 @@
         <v>1.222172323089755</v>
       </c>
       <c r="L18">
+        <f t="shared" si="6"/>
+        <v>1287.9591836734694</v>
+      </c>
+      <c r="M18">
         <f t="shared" si="4"/>
-        <v>1287.9591836734694</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>15.240000000000009</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="5"/>
+        <v>1.222172323089755</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -9530,20 +9966,28 @@
         <v>8.5231586940015234</v>
       </c>
       <c r="L19">
+        <f t="shared" si="6"/>
+        <v>192.76</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="4"/>
-        <v>192.76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>4.490000000000002</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="5"/>
+        <v>8.5231586940015234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:14">
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:14">
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:14">
       <c r="J23" s="5" t="s">
         <v>16</v>
       </c>
@@ -9552,7 +9996,7 @@
         <v>10.026</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:14">
       <c r="J24" s="5" t="s">
         <v>15</v>
       </c>
@@ -9561,7 +10005,7 @@
         <v>8.7369450758959371</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:14">
       <c r="J25" s="5" t="s">
         <v>17</v>
       </c>
@@ -9570,26 +10014,75 @@
         <v>11.163236069151344</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:14">
       <c r="J26" s="5"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:12">
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="K28" s="3"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="K29" s="3"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="K30" s="3"/>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="K31" s="3"/>
-    </row>
-    <row r="32" spans="1:12">
+    <row r="27" spans="1:14">
+      <c r="I27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27">
+        <f>AVERAGE(J5:J19)</f>
+        <v>10.026</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M27">
+        <f>AVERAGE(M5:M19)</f>
+        <v>5.9091666666666613</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="I28" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28">
+        <f>STDEV(J5:J19)</f>
+        <v>10.362471988588714</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M28">
+        <f>STDEV(M5:M19)</f>
+        <v>5.396376660371855</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="J30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30">
+        <f>AVERAGE(K5:K18)</f>
+        <v>8.7522155317455379</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N30">
+        <f>AVERAGE(N5:N19)</f>
+        <v>4.3431662129137703</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="J31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K31">
+        <f>STDEV(K5:K19)</f>
+        <v>12.599357815423968</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N31">
+        <f>STDEV(N5:N19)</f>
+        <v>5.2150735335977192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="K32" s="3"/>
     </row>
     <row r="33" spans="11:11">

</xml_diff>

<commit_message>
minor edits to calib and measure
</commit_message>
<xml_diff>
--- a/software/ble/Calib_and_Measure.xlsx
+++ b/software/ble/Calib_and_Measure.xlsx
@@ -196,8 +196,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -217,13 +219,15 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -490,11 +494,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2141612856"/>
-        <c:axId val="2141615784"/>
+        <c:axId val="-2129880216"/>
+        <c:axId val="-2129877288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2141612856"/>
+        <c:axId val="-2129880216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -504,12 +508,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141615784"/>
+        <c:crossAx val="-2129877288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141615784"/>
+        <c:axId val="-2129877288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,7 +524,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141612856"/>
+        <c:crossAx val="-2129880216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -594,46 +598,46 @@
                   <c:v>163.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108.58</c:v>
+                  <c:v>108.22</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>236.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>827.87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1246.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1729.73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>306.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>197.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>129.47</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.33</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52.27</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>108.58</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>55.28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>306.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>47.49</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>108.22</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>197.09</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>129.47</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>51.08</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.33</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1729.73</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>827.87</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1246.96</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>52.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -648,46 +652,46 @@
                   <c:v>0.989999999999981</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.97</c:v>
+                  <c:v>5.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.95999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>22.11000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.24000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.00999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.930000000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.509999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.030000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.999999999999986</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.829999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.619999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.490000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>36.97</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>20.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.930000000000007</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.509999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.299999999999997</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.030000000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.999999999999986</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.829999999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.619999999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>16.00999999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>22.11000000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15.24000000000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.490000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -702,11 +706,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2053272696"/>
-        <c:axId val="2053269736"/>
+        <c:axId val="-2127857800"/>
+        <c:axId val="-2127854792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2053272696"/>
+        <c:axId val="-2127857800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -716,12 +720,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2053269736"/>
+        <c:crossAx val="-2127854792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2053269736"/>
+        <c:axId val="-2127854792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -732,7 +736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2053272696"/>
+        <c:crossAx val="-2127857800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -807,46 +811,46 @@
                   <c:v>163.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108.58</c:v>
+                  <c:v>108.22</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>236.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>827.87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1246.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1729.73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>306.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>197.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>129.47</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.33</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52.27</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>108.58</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>55.28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>306.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>47.49</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>108.22</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>197.09</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>129.47</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>51.08</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.33</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1729.73</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>827.87</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1246.96</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>52.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -861,46 +865,46 @@
                   <c:v>0.610470493926115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.67129325705712</c:v>
+                  <c:v>4.89743115875069</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.258449895837753</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2.670709169314024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.222172323089755</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.92557798037844</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.631668521306541</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.57998764669549</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.601742852774806</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.08856458960697</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.64551942902458</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.80570801317233</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.523158694001523</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>34.67129325705712</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>39.92172211350293</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.631668521306541</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19.57998764669549</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.89743115875069</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.601742852774806</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.08856458960697</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.64551942902458</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.80570801317233</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.92557798037844</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.670709169314024</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.222172323089755</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>8.523158694001523</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -915,11 +919,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2053242728"/>
-        <c:axId val="2053239768"/>
+        <c:axId val="-2127823672"/>
+        <c:axId val="-2127820712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2053242728"/>
+        <c:axId val="-2127823672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -929,12 +933,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2053239768"/>
+        <c:crossAx val="-2127820712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2053239768"/>
+        <c:axId val="-2127820712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22.0"/>
@@ -946,7 +950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2053242728"/>
+        <c:crossAx val="-2127823672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1335,8 +1339,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2141708664"/>
-        <c:axId val="2141711656"/>
+        <c:axId val="-2129777096"/>
+        <c:axId val="-2129774104"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1514,11 +1518,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2141717928"/>
-        <c:axId val="2141714984"/>
+        <c:axId val="-2129767832"/>
+        <c:axId val="-2129770776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2141708664"/>
+        <c:axId val="-2129777096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1528,12 +1532,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141711656"/>
+        <c:crossAx val="-2129774104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141711656"/>
+        <c:axId val="-2129774104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600.0"/>
@@ -1546,12 +1550,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141708664"/>
+        <c:crossAx val="-2129777096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141714984"/>
+        <c:axId val="-2129770776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1563,12 +1567,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141717928"/>
+        <c:crossAx val="-2129767832"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141717928"/>
+        <c:axId val="-2129767832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1578,7 +1582,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141714984"/>
+        <c:crossAx val="-2129770776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2077,8 +2081,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2141764280"/>
-        <c:axId val="2141769672"/>
+        <c:axId val="-2129721192"/>
+        <c:axId val="-2129715800"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2316,11 +2320,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2141775944"/>
-        <c:axId val="2141773000"/>
+        <c:axId val="-2129709528"/>
+        <c:axId val="-2129712472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2141764280"/>
+        <c:axId val="-2129721192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2330,12 +2334,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141769672"/>
+        <c:crossAx val="-2129715800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141769672"/>
+        <c:axId val="-2129715800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2346,12 +2350,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141764280"/>
+        <c:crossAx val="-2129721192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141773000"/>
+        <c:axId val="-2129712472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -2363,12 +2367,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141775944"/>
+        <c:crossAx val="-2129709528"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141775944"/>
+        <c:axId val="-2129709528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2378,7 +2382,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141773000"/>
+        <c:crossAx val="-2129712472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2643,11 +2647,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2141796184"/>
-        <c:axId val="2141799144"/>
+        <c:axId val="-2129689288"/>
+        <c:axId val="-2129686328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2141796184"/>
+        <c:axId val="-2129689288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2657,12 +2661,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141799144"/>
+        <c:crossAx val="-2129686328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141799144"/>
+        <c:axId val="-2129686328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50.0"/>
@@ -2674,7 +2678,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141796184"/>
+        <c:crossAx val="-2129689288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2939,11 +2943,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2053996856"/>
-        <c:axId val="2053999816"/>
+        <c:axId val="-2130681256"/>
+        <c:axId val="-2130684216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2053996856"/>
+        <c:axId val="-2130681256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2953,12 +2957,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2053999816"/>
+        <c:crossAx val="-2130684216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2053999816"/>
+        <c:axId val="-2130684216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22.0"/>
@@ -2970,7 +2974,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2053996856"/>
+        <c:crossAx val="-2130681256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3469,8 +3473,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2054059912"/>
-        <c:axId val="2054065304"/>
+        <c:axId val="-2127488952"/>
+        <c:axId val="-2127483560"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3708,11 +3712,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2054071576"/>
-        <c:axId val="2054068632"/>
+        <c:axId val="-2127477288"/>
+        <c:axId val="-2127480232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2054059912"/>
+        <c:axId val="-2127488952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3722,12 +3726,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2054065304"/>
+        <c:crossAx val="-2127483560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2054065304"/>
+        <c:axId val="-2127483560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3738,12 +3742,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2054059912"/>
+        <c:crossAx val="-2127488952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2054068632"/>
+        <c:axId val="-2127480232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -3755,12 +3759,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2054071576"/>
+        <c:crossAx val="-2127477288"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2054071576"/>
+        <c:axId val="-2127477288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3770,7 +3774,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2054068632"/>
+        <c:crossAx val="-2127480232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4037,11 +4041,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2054092776"/>
-        <c:axId val="2054095736"/>
+        <c:axId val="-2127456424"/>
+        <c:axId val="-2127453464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2054092776"/>
+        <c:axId val="-2127456424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4051,12 +4055,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2054095736"/>
+        <c:crossAx val="-2127453464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2054095736"/>
+        <c:axId val="-2127453464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4067,7 +4071,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2054092776"/>
+        <c:crossAx val="-2127456424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4334,11 +4338,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2054123704"/>
-        <c:axId val="2054126664"/>
+        <c:axId val="-2127426056"/>
+        <c:axId val="-2127423096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2054123704"/>
+        <c:axId val="-2127426056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4348,12 +4352,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2054126664"/>
+        <c:crossAx val="-2127423096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2054126664"/>
+        <c:axId val="-2127423096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22.0"/>
@@ -4365,7 +4369,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2054123704"/>
+        <c:crossAx val="-2127426056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4448,46 +4452,46 @@
                   <c:v>163.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108.58</c:v>
+                  <c:v>108.22</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>236.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>827.87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1246.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1729.73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>306.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>197.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>129.47</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.33</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52.27</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>108.58</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>55.28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>306.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>47.49</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>108.22</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>197.09</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>129.47</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>51.08</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.33</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1729.73</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>827.87</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1246.96</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>52.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4502,46 +4506,46 @@
                   <c:v>161.18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>143.6</c:v>
+                  <c:v>102.92</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>238.17</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>805.76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1262.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1745.74</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>303.61</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39.06</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>187.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>125.51</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49.61</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.49</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>48.19</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>143.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>71.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>303.61</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>39.06</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>102.92</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>187.2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>125.51</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>49.61</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.49</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1745.74</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>805.76</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1262.2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>48.19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4589,46 +4593,46 @@
                   <c:v>163.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108.58</c:v>
+                  <c:v>108.22</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>236.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>827.87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1246.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1729.73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>306.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>197.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>129.47</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.33</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52.27</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>108.58</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>55.28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>306.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>47.49</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>108.22</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>197.09</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>129.47</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>51.08</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.33</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1729.73</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>827.87</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1246.96</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>52.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4642,35 +4646,35 @@
                 <c:pt idx="0">
                   <c:v>162.17</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>106.63</c:v>
-                </c:pt>
                 <c:pt idx="2">
                   <c:v>235.21</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
+                  <c:v>305.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48.57</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>196.23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>129.51</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.44</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52.68</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>106.63</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>51.1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>305.54</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>48.57</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>196.23</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>129.51</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50.44</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.11</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>52.68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4685,8 +4689,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2053302616"/>
-        <c:axId val="2053300056"/>
+        <c:axId val="-2127370568"/>
+        <c:axId val="-2127365160"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4732,46 +4736,46 @@
                   <c:v>163.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108.58</c:v>
+                  <c:v>108.22</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>236.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>827.87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1246.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1729.73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>306.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>197.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>129.47</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.33</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52.27</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>108.58</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>55.28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>306.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>47.49</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>108.22</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>197.09</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>129.47</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>51.08</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.33</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1729.73</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>827.87</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1246.96</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>52.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4786,46 +4790,46 @@
                   <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>0.28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.77</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.19</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.44</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.48</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.91</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.96</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.98</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4840,11 +4844,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2053293784"/>
-        <c:axId val="2053296728"/>
+        <c:axId val="-2127358888"/>
+        <c:axId val="-2127361832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2053302616"/>
+        <c:axId val="-2127370568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4854,12 +4858,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2053300056"/>
+        <c:crossAx val="-2127365160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2053300056"/>
+        <c:axId val="-2127365160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4870,12 +4874,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2053302616"/>
+        <c:crossAx val="-2127370568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2053296728"/>
+        <c:axId val="-2127361832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -4887,12 +4891,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2053293784"/>
+        <c:crossAx val="-2127358888"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2053293784"/>
+        <c:axId val="-2127358888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4902,7 +4906,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2053296728"/>
+        <c:crossAx val="-2127361832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7452,7 +7456,7 @@
   <dimension ref="A1:AE44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40:J44"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9189,7 +9193,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG34" sqref="AG34"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9286,11 +9290,11 @@
         <v>0.98999999999998067</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" ref="K5:K19" si="0">J5/I5*100</f>
+        <f>J5/I5*100</f>
         <v>0.61047049392611508</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L10" si="1">F5/G5</f>
+        <f>F5/G5</f>
         <v>255.84126984126985</v>
       </c>
       <c r="M5">
@@ -9304,52 +9308,46 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>106.63</v>
-      </c>
-      <c r="C6">
-        <v>0.49</v>
+        <v>28</v>
       </c>
       <c r="D6">
-        <v>108.58</v>
+        <v>108.22</v>
       </c>
       <c r="E6">
-        <v>0.49</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>143.6</v>
+        <v>102.92</v>
       </c>
       <c r="G6">
-        <v>0.5</v>
+        <v>0.44</v>
       </c>
       <c r="H6">
-        <v>26.77</v>
+        <v>8.07</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I19" si="2">IF(B6&gt;0,B6,D6)</f>
-        <v>106.63</v>
+        <f>IF(B6&gt;0,B6,D6)</f>
+        <v>108.22</v>
       </c>
       <c r="J6">
-        <f t="shared" ref="J6:J19" si="3">ABS(I6-F6)</f>
-        <v>36.97</v>
+        <f>ABS(I6-F6)</f>
+        <v>5.2999999999999972</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="0"/>
-        <v>34.671293257057116</v>
+        <f>J6/I6*100</f>
+        <v>4.89743115875069</v>
       </c>
       <c r="L6">
-        <f t="shared" si="1"/>
-        <v>287.2</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" ref="M6:M19" si="4">IF(J6&gt;(J$27+J$28),"",J6)</f>
-        <v/>
-      </c>
-      <c r="N6" t="str">
-        <f t="shared" ref="N6:N19" si="5">IF(K6&gt;(K$30+K$31),"",K6)</f>
-        <v/>
+        <f>F6/G6</f>
+        <v>233.90909090909091</v>
+      </c>
+      <c r="M6">
+        <f>IF(J6&gt;(J$27+J$28),"",J6)</f>
+        <v>5.2999999999999972</v>
+      </c>
+      <c r="N6">
+        <f>IF(K6&gt;(K$30+K$31),"",K6)</f>
+        <v>4.89743115875069</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -9378,604 +9376,610 @@
         <v>1.71</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f>IF(B7&gt;0,B7,D7)</f>
         <v>235.21</v>
       </c>
       <c r="J7">
-        <f t="shared" si="3"/>
+        <f>ABS(I7-F7)</f>
         <v>2.9599999999999795</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="0"/>
+        <f>J7/I7*100</f>
         <v>1.2584498958377532</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
+        <f>F7/G7</f>
         <v>309.31168831168827</v>
       </c>
       <c r="M7">
-        <f t="shared" si="4"/>
+        <f>IF(J7&gt;(J$27+J$28),"",J7)</f>
         <v>2.9599999999999795</v>
       </c>
       <c r="N7">
-        <f t="shared" si="5"/>
+        <f>IF(K7&gt;(K$30+K$31),"",K7)</f>
         <v>1.2584498958377532</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8">
-        <v>51.1</v>
-      </c>
-      <c r="C8">
-        <v>0.3</v>
+        <v>35</v>
       </c>
       <c r="D8">
-        <v>55.28</v>
+        <v>827.87</v>
       </c>
       <c r="E8">
-        <v>0.32</v>
+        <v>0.99</v>
       </c>
       <c r="F8">
-        <v>71.5</v>
+        <v>805.76</v>
       </c>
       <c r="G8">
-        <v>0.28000000000000003</v>
+        <v>0.96</v>
       </c>
       <c r="H8">
-        <v>40.06</v>
+        <v>12.09</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
-        <v>51.1</v>
+        <f>IF(B8&gt;0,B8,D8)</f>
+        <v>827.87</v>
       </c>
       <c r="J8">
-        <f t="shared" si="3"/>
-        <v>20.399999999999999</v>
+        <f>ABS(I8-F8)</f>
+        <v>22.110000000000014</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="0"/>
-        <v>39.921722113502931</v>
+        <f>J8/I8*100</f>
+        <v>2.6707091693140246</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
-        <v>255.35714285714283</v>
+        <f>F8/G8</f>
+        <v>839.33333333333337</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(J8&gt;(J$27+J$28),"",J8)</f>
         <v/>
       </c>
-      <c r="N8" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+      <c r="N8">
+        <f>IF(K8&gt;(K$30+K$31),"",K8)</f>
+        <v>2.6707091693140246</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9">
-        <v>305.54000000000002</v>
-      </c>
-      <c r="C9">
-        <v>0.83</v>
+        <v>34</v>
       </c>
       <c r="D9">
-        <v>306.42</v>
+        <v>1246.96</v>
       </c>
       <c r="E9">
-        <v>0.83</v>
+        <v>0.98</v>
       </c>
       <c r="F9">
-        <v>303.61</v>
+        <v>1262.2</v>
       </c>
       <c r="G9">
-        <v>0.77</v>
+        <v>0.98</v>
       </c>
       <c r="H9">
-        <v>69.489999999999995</v>
+        <v>24.57</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
-        <v>305.54000000000002</v>
+        <f>IF(B9&gt;0,B9,D9)</f>
+        <v>1246.96</v>
       </c>
       <c r="J9">
-        <f t="shared" si="3"/>
-        <v>1.9300000000000068</v>
+        <f>ABS(I9-F9)</f>
+        <v>15.240000000000009</v>
       </c>
       <c r="K9" s="3">
-        <f t="shared" si="0"/>
-        <v>0.63166852130654139</v>
+        <f>J9/I9*100</f>
+        <v>1.222172323089755</v>
       </c>
       <c r="L9">
-        <f t="shared" si="1"/>
-        <v>394.2987012987013</v>
+        <f>F9/G9</f>
+        <v>1287.9591836734694</v>
       </c>
       <c r="M9">
-        <f t="shared" si="4"/>
-        <v>1.9300000000000068</v>
+        <f>IF(J9&gt;(J$27+J$28),"",J9)</f>
+        <v>15.240000000000009</v>
       </c>
       <c r="N9">
-        <f t="shared" si="5"/>
-        <v>0.63166852130654139</v>
+        <f>IF(K9&gt;(K$30+K$31),"",K9)</f>
+        <v>1.222172323089755</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10">
-        <v>48.57</v>
-      </c>
-      <c r="C10">
-        <v>0.61</v>
+        <v>36</v>
       </c>
       <c r="D10">
-        <v>47.49</v>
+        <v>1729.73</v>
       </c>
       <c r="E10">
-        <v>0.62</v>
+        <v>0.92</v>
       </c>
       <c r="F10">
-        <v>39.06</v>
+        <v>1745.74</v>
       </c>
       <c r="G10">
-        <v>0.19</v>
+        <v>0.91</v>
       </c>
       <c r="H10">
-        <v>17.329999999999998</v>
+        <v>238.36</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
-        <v>48.57</v>
+        <f>IF(B10&gt;0,B10,D10)</f>
+        <v>1729.73</v>
       </c>
       <c r="J10">
-        <f t="shared" si="3"/>
-        <v>9.509999999999998</v>
+        <f>ABS(I10-F10)</f>
+        <v>16.009999999999991</v>
       </c>
       <c r="K10" s="3">
-        <f t="shared" si="0"/>
-        <v>19.579987646695489</v>
+        <f>J10/I10*100</f>
+        <v>0.92557798037844008</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
-        <v>205.57894736842107</v>
+        <f>F10/G10</f>
+        <v>1918.3956043956043</v>
       </c>
       <c r="M10">
-        <f t="shared" si="4"/>
-        <v>9.509999999999998</v>
+        <f>IF(J10&gt;(J$27+J$28),"",J10)</f>
+        <v>16.009999999999991</v>
       </c>
       <c r="N10">
-        <f t="shared" si="5"/>
-        <v>19.579987646695489</v>
+        <f>IF(K10&gt;(K$30+K$31),"",K10)</f>
+        <v>0.92557798037844008</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>305.54000000000002</v>
+      </c>
+      <c r="C11">
+        <v>0.83</v>
       </c>
       <c r="D11">
-        <v>108.22</v>
+        <v>306.42</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="F11">
-        <v>102.92</v>
+        <v>303.61</v>
       </c>
       <c r="G11">
-        <v>0.44</v>
+        <v>0.77</v>
       </c>
       <c r="H11">
-        <v>8.07</v>
+        <v>69.489999999999995</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
-        <v>108.22</v>
+        <f>IF(B11&gt;0,B11,D11)</f>
+        <v>305.54000000000002</v>
       </c>
       <c r="J11">
-        <f t="shared" si="3"/>
-        <v>5.2999999999999972</v>
+        <f>ABS(I11-F11)</f>
+        <v>1.9300000000000068</v>
       </c>
       <c r="K11" s="3">
-        <f t="shared" si="0"/>
-        <v>4.89743115875069</v>
+        <f>J11/I11*100</f>
+        <v>0.63166852130654139</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11:L19" si="6">F11/G11</f>
-        <v>233.90909090909091</v>
+        <f>F11/G11</f>
+        <v>394.2987012987013</v>
       </c>
       <c r="M11">
-        <f t="shared" si="4"/>
-        <v>5.2999999999999972</v>
+        <f>IF(J11&gt;(J$27+J$28),"",J11)</f>
+        <v>1.9300000000000068</v>
       </c>
       <c r="N11">
-        <f t="shared" si="5"/>
-        <v>4.89743115875069</v>
+        <f>IF(K11&gt;(K$30+K$31),"",K11)</f>
+        <v>0.63166852130654139</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12">
-        <v>196.23</v>
+        <v>48.57</v>
       </c>
       <c r="C12">
-        <v>0.62</v>
+        <v>0.61</v>
       </c>
       <c r="D12">
-        <v>197.09</v>
+        <v>47.49</v>
       </c>
       <c r="E12">
         <v>0.62</v>
       </c>
       <c r="F12">
-        <v>187.2</v>
+        <v>39.06</v>
       </c>
       <c r="G12">
-        <v>0.48</v>
+        <v>0.19</v>
       </c>
       <c r="H12">
-        <v>152.66999999999999</v>
+        <v>17.329999999999998</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
-        <v>196.23</v>
+        <f>IF(B12&gt;0,B12,D12)</f>
+        <v>48.57</v>
       </c>
       <c r="J12">
-        <f t="shared" si="3"/>
-        <v>9.0300000000000011</v>
+        <f>ABS(I12-F12)</f>
+        <v>9.509999999999998</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" si="0"/>
-        <v>4.6017428527748061</v>
+        <f>J12/I12*100</f>
+        <v>19.579987646695489</v>
       </c>
       <c r="L12">
-        <f t="shared" si="6"/>
-        <v>390</v>
+        <f>F12/G12</f>
+        <v>205.57894736842107</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
-        <v>9.0300000000000011</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="5"/>
-        <v>4.6017428527748061</v>
+        <f>IF(J12&gt;(J$27+J$28),"",J12)</f>
+        <v>9.509999999999998</v>
+      </c>
+      <c r="N12" t="str">
+        <f>IF(K12&gt;(K$30+K$31),"",K12)</f>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13">
-        <v>129.51</v>
+        <v>196.23</v>
       </c>
       <c r="C13">
-        <v>0.61</v>
+        <v>0.62</v>
       </c>
       <c r="D13">
-        <v>129.47</v>
+        <v>197.09</v>
       </c>
       <c r="E13">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="F13">
-        <v>125.51</v>
+        <v>187.2</v>
       </c>
       <c r="G13">
-        <v>0.45</v>
+        <v>0.48</v>
       </c>
       <c r="H13">
-        <v>24.11</v>
+        <v>152.66999999999999</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
-        <v>129.51</v>
+        <f>IF(B13&gt;0,B13,D13)</f>
+        <v>196.23</v>
       </c>
       <c r="J13">
-        <f t="shared" si="3"/>
-        <v>3.9999999999999858</v>
+        <f>ABS(I13-F13)</f>
+        <v>9.0300000000000011</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" si="0"/>
-        <v>3.0885645896069693</v>
+        <f>J13/I13*100</f>
+        <v>4.6017428527748061</v>
       </c>
       <c r="L13">
-        <f t="shared" si="6"/>
-        <v>278.9111111111111</v>
+        <f>F13/G13</f>
+        <v>390</v>
       </c>
       <c r="M13">
-        <f t="shared" si="4"/>
-        <v>3.9999999999999858</v>
+        <f>IF(J13&gt;(J$27+J$28),"",J13)</f>
+        <v>9.0300000000000011</v>
       </c>
       <c r="N13">
-        <f t="shared" si="5"/>
-        <v>3.0885645896069693</v>
+        <f>IF(K13&gt;(K$30+K$31),"",K13)</f>
+        <v>4.6017428527748061</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14">
-        <v>50.44</v>
+        <v>129.51</v>
       </c>
       <c r="C14">
-        <v>0.56999999999999995</v>
+        <v>0.61</v>
       </c>
       <c r="D14">
-        <v>51.08</v>
+        <v>129.47</v>
       </c>
       <c r="E14">
-        <v>0.57999999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="F14">
-        <v>49.61</v>
+        <v>125.51</v>
       </c>
       <c r="G14">
-        <v>0.22</v>
+        <v>0.45</v>
       </c>
       <c r="H14">
-        <v>10.46</v>
+        <v>24.11</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
-        <v>50.44</v>
+        <f>IF(B14&gt;0,B14,D14)</f>
+        <v>129.51</v>
       </c>
       <c r="J14">
-        <f t="shared" si="3"/>
-        <v>0.82999999999999829</v>
+        <f>ABS(I14-F14)</f>
+        <v>3.9999999999999858</v>
       </c>
       <c r="K14" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6455194290245803</v>
+        <f>J14/I14*100</f>
+        <v>3.0885645896069693</v>
       </c>
       <c r="L14">
-        <f t="shared" si="6"/>
-        <v>225.5</v>
+        <f>F14/G14</f>
+        <v>278.9111111111111</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
-        <v>0.82999999999999829</v>
+        <f>IF(J14&gt;(J$27+J$28),"",J14)</f>
+        <v>3.9999999999999858</v>
       </c>
       <c r="N14">
-        <f t="shared" si="5"/>
-        <v>1.6455194290245803</v>
+        <f>IF(K14&gt;(K$30+K$31),"",K14)</f>
+        <v>3.0885645896069693</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15">
-        <v>9.11</v>
+        <v>50.44</v>
       </c>
       <c r="C15">
-        <v>0.46</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="D15">
-        <v>9.33</v>
+        <v>51.08</v>
       </c>
       <c r="E15">
-        <v>0.56999999999999995</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="F15">
-        <v>8.49</v>
+        <v>49.61</v>
       </c>
       <c r="G15">
-        <v>0.06</v>
+        <v>0.22</v>
       </c>
       <c r="H15">
-        <v>2.31</v>
+        <v>10.46</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
-        <v>9.11</v>
+        <f>IF(B15&gt;0,B15,D15)</f>
+        <v>50.44</v>
       </c>
       <c r="J15">
-        <f t="shared" si="3"/>
-        <v>0.61999999999999922</v>
+        <f>ABS(I15-F15)</f>
+        <v>0.82999999999999829</v>
       </c>
       <c r="K15" s="3">
-        <f t="shared" si="0"/>
-        <v>6.8057080131723309</v>
+        <f>J15/I15*100</f>
+        <v>1.6455194290245803</v>
       </c>
       <c r="L15">
-        <f t="shared" si="6"/>
-        <v>141.5</v>
+        <f>F15/G15</f>
+        <v>225.5</v>
       </c>
       <c r="M15">
-        <f t="shared" si="4"/>
-        <v>0.61999999999999922</v>
+        <f>IF(J15&gt;(J$27+J$28),"",J15)</f>
+        <v>0.82999999999999829</v>
       </c>
       <c r="N15">
-        <f t="shared" si="5"/>
-        <v>6.8057080131723309</v>
+        <f>IF(K15&gt;(K$30+K$31),"",K15)</f>
+        <v>1.6455194290245803</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>9.11</v>
+      </c>
+      <c r="C16">
+        <v>0.46</v>
       </c>
       <c r="D16">
-        <v>1729.73</v>
+        <v>9.33</v>
       </c>
       <c r="E16">
-        <v>0.92</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F16">
-        <v>1745.74</v>
+        <v>8.49</v>
       </c>
       <c r="G16">
-        <v>0.91</v>
+        <v>0.06</v>
       </c>
       <c r="H16">
-        <v>238.36</v>
+        <v>2.31</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
-        <v>1729.73</v>
+        <f>IF(B16&gt;0,B16,D16)</f>
+        <v>9.11</v>
       </c>
       <c r="J16">
-        <f t="shared" si="3"/>
-        <v>16.009999999999991</v>
+        <f>ABS(I16-F16)</f>
+        <v>0.61999999999999922</v>
       </c>
       <c r="K16" s="3">
-        <f t="shared" si="0"/>
-        <v>0.92557798037844008</v>
+        <f>J16/I16*100</f>
+        <v>6.8057080131723309</v>
       </c>
       <c r="L16">
-        <f t="shared" si="6"/>
-        <v>1918.3956043956043</v>
+        <f>F16/G16</f>
+        <v>141.5</v>
       </c>
       <c r="M16">
-        <f t="shared" si="4"/>
-        <v>16.009999999999991</v>
+        <f>IF(J16&gt;(J$27+J$28),"",J16)</f>
+        <v>0.61999999999999922</v>
       </c>
       <c r="N16">
-        <f t="shared" si="5"/>
-        <v>0.92557798037844008</v>
+        <f>IF(K16&gt;(K$30+K$31),"",K16)</f>
+        <v>6.8057080131723309</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>52.68</v>
+      </c>
+      <c r="C17">
+        <v>0.51</v>
       </c>
       <c r="D17">
-        <v>827.87</v>
+        <v>52.27</v>
       </c>
       <c r="E17">
-        <v>0.99</v>
+        <v>0.51</v>
       </c>
       <c r="F17">
-        <v>805.76</v>
+        <v>48.19</v>
       </c>
       <c r="G17">
-        <v>0.96</v>
+        <v>0.25</v>
       </c>
       <c r="H17">
-        <v>12.09</v>
+        <v>4.91</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
-        <v>827.87</v>
+        <f>IF(B17&gt;0,B17,D17)</f>
+        <v>52.68</v>
       </c>
       <c r="J17">
-        <f t="shared" si="3"/>
-        <v>22.110000000000014</v>
+        <f>ABS(I17-F17)</f>
+        <v>4.490000000000002</v>
       </c>
       <c r="K17" s="3">
-        <f t="shared" si="0"/>
-        <v>2.6707091693140246</v>
+        <f>J17/I17*100</f>
+        <v>8.5231586940015234</v>
       </c>
       <c r="L17">
-        <f t="shared" si="6"/>
-        <v>839.33333333333337</v>
-      </c>
-      <c r="M17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f>F17/G17</f>
+        <v>192.76</v>
+      </c>
+      <c r="M17">
+        <f>IF(J17&gt;(J$27+J$28),"",J17)</f>
+        <v>4.490000000000002</v>
       </c>
       <c r="N17">
-        <f t="shared" si="5"/>
-        <v>2.6707091693140246</v>
+        <f>IF(K17&gt;(K$30+K$31),"",K17)</f>
+        <v>8.5231586940015234</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>106.63</v>
+      </c>
+      <c r="C18">
+        <v>0.49</v>
       </c>
       <c r="D18">
-        <v>1246.96</v>
+        <v>108.58</v>
       </c>
       <c r="E18">
-        <v>0.98</v>
+        <v>0.49</v>
       </c>
       <c r="F18">
-        <v>1262.2</v>
+        <v>143.6</v>
       </c>
       <c r="G18">
-        <v>0.98</v>
+        <v>0.5</v>
       </c>
       <c r="H18">
-        <v>24.57</v>
+        <v>26.77</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
-        <v>1246.96</v>
+        <f>IF(B18&gt;0,B18,D18)</f>
+        <v>106.63</v>
       </c>
       <c r="J18">
-        <f t="shared" si="3"/>
-        <v>15.240000000000009</v>
+        <f>ABS(I18-F18)</f>
+        <v>36.97</v>
       </c>
       <c r="K18" s="3">
-        <f t="shared" si="0"/>
-        <v>1.222172323089755</v>
+        <f>J18/I18*100</f>
+        <v>34.671293257057116</v>
       </c>
       <c r="L18">
-        <f t="shared" si="6"/>
-        <v>1287.9591836734694</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="4"/>
-        <v>15.240000000000009</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="5"/>
-        <v>1.222172323089755</v>
+        <f>F18/G18</f>
+        <v>287.2</v>
+      </c>
+      <c r="M18" t="str">
+        <f>IF(J18&gt;(J$27+J$28),"",J18)</f>
+        <v/>
+      </c>
+      <c r="N18" t="str">
+        <f>IF(K18&gt;(K$30+K$31),"",K18)</f>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B19">
-        <v>52.68</v>
+        <v>51.1</v>
       </c>
       <c r="C19">
-        <v>0.51</v>
+        <v>0.3</v>
       </c>
       <c r="D19">
-        <v>52.27</v>
+        <v>55.28</v>
       </c>
       <c r="E19">
-        <v>0.51</v>
+        <v>0.32</v>
       </c>
       <c r="F19">
-        <v>48.19</v>
+        <v>71.5</v>
       </c>
       <c r="G19">
-        <v>0.25</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H19">
-        <v>4.91</v>
+        <v>40.06</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
-        <v>52.68</v>
+        <f>IF(B19&gt;0,B19,D19)</f>
+        <v>51.1</v>
       </c>
       <c r="J19">
-        <f t="shared" si="3"/>
-        <v>4.490000000000002</v>
+        <f>ABS(I19-F19)</f>
+        <v>20.399999999999999</v>
       </c>
       <c r="K19" s="3">
-        <f t="shared" si="0"/>
-        <v>8.5231586940015234</v>
+        <f>J19/I19*100</f>
+        <v>39.921722113502931</v>
       </c>
       <c r="L19">
-        <f t="shared" si="6"/>
-        <v>192.76</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="4"/>
-        <v>4.490000000000002</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="5"/>
-        <v>8.5231586940015234</v>
+        <f>F19/G19</f>
+        <v>255.35714285714283</v>
+      </c>
+      <c r="M19" t="str">
+        <f>IF(J19&gt;(J$27+J$28),"",J19)</f>
+        <v/>
+      </c>
+      <c r="N19" t="str">
+        <f>IF(K19&gt;(K$30+K$31),"",K19)</f>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -10056,14 +10060,14 @@
       </c>
       <c r="K30">
         <f>AVERAGE(K5:K18)</f>
-        <v>8.7522155317455379</v>
+        <v>6.5094610017811521</v>
       </c>
       <c r="M30" s="5" t="s">
         <v>38</v>
       </c>
       <c r="N30">
         <f>AVERAGE(N5:N19)</f>
-        <v>4.3431662129137703</v>
+        <v>3.0734310934319615</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -10079,7 +10083,7 @@
       </c>
       <c r="N31">
         <f>STDEV(N5:N19)</f>
-        <v>5.2150735335977192</v>
+        <v>2.6086647375321572</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -10089,6 +10093,9 @@
       <c r="K33" s="3"/>
     </row>
   </sheetData>
+  <sortState ref="A4:N19">
+    <sortCondition descending="1" ref="E4:E19"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>

</xml_diff>